<commit_message>
enhance orphan matches with summary vectorization via SBERT
</commit_message>
<xml_diff>
--- a/top_clusters.xlsx
+++ b/top_clusters.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Top100" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Top100" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -447,7 +447,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T109"/>
+  <dimension ref="A1:T108"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1388,11 +1388,11 @@
         </is>
       </c>
       <c r="E13" t="n">
-        <v>100015333</v>
+        <v>100016342</v>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>100015333:0:0</t>
+          <t>100016342:2:0</t>
         </is>
       </c>
       <c r="G13" t="n">
@@ -1426,11 +1426,6 @@
       </c>
       <c r="N13" t="n">
         <v>63</v>
-      </c>
-      <c r="O13" t="inlineStr">
-        <is>
-          <t>male</t>
-        </is>
       </c>
       <c r="P13" t="n">
         <v>38.9072362908274</v>
@@ -1468,11 +1463,11 @@
         </is>
       </c>
       <c r="E14" t="n">
-        <v>100016342</v>
+        <v>100015333</v>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>100016342:2:0</t>
+          <t>100015333:0:0</t>
         </is>
       </c>
       <c r="G14" t="n">
@@ -1506,6 +1501,11 @@
       </c>
       <c r="N14" t="n">
         <v>63</v>
+      </c>
+      <c r="O14" t="inlineStr">
+        <is>
+          <t>male</t>
+        </is>
       </c>
       <c r="P14" t="n">
         <v>38.9072362908274</v>
@@ -2028,11 +2028,11 @@
         </is>
       </c>
       <c r="E21" t="n">
-        <v>100000119</v>
+        <v>100068117</v>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>100000119:0:0</t>
+          <t>100068117:0:0</t>
         </is>
       </c>
       <c r="G21" t="n">
@@ -2073,14 +2073,14 @@
         </is>
       </c>
       <c r="P21" t="n">
-        <v>38.88682291</v>
+        <v>38.887589465233</v>
       </c>
       <c r="Q21" t="n">
-        <v>-76.97917206</v>
+        <v>-76.98076325387819</v>
       </c>
       <c r="R21" t="inlineStr">
         <is>
-          <t>1740 BAY STREET SE</t>
+          <t>17TH STREET SE AND INDEPENDENCE AVENUE SE</t>
         </is>
       </c>
       <c r="S21" t="inlineStr">
@@ -2113,11 +2113,11 @@
         </is>
       </c>
       <c r="E22" t="n">
-        <v>100068117</v>
+        <v>100000119</v>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>100068117:0:0</t>
+          <t>100000119:0:0</t>
         </is>
       </c>
       <c r="G22" t="n">
@@ -2158,14 +2158,14 @@
         </is>
       </c>
       <c r="P22" t="n">
-        <v>38.887589465233</v>
+        <v>38.88682291</v>
       </c>
       <c r="Q22" t="n">
-        <v>-76.98076325387819</v>
+        <v>-76.97917206</v>
       </c>
       <c r="R22" t="inlineStr">
         <is>
-          <t>17TH STREET SE AND INDEPENDENCE AVENUE SE</t>
+          <t>1740 BAY STREET SE</t>
         </is>
       </c>
       <c r="S22" t="inlineStr">
@@ -2442,11 +2442,11 @@
         </is>
       </c>
       <c r="E26" t="n">
-        <v>100015333</v>
+        <v>100016342</v>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>100015333:1:0</t>
+          <t>100016342:1:0</t>
         </is>
       </c>
       <c r="G26" t="n">
@@ -2486,17 +2486,6 @@
           <t>male</t>
         </is>
       </c>
-      <c r="P26" t="n">
-        <v>38.9072362908274</v>
-      </c>
-      <c r="Q26" t="n">
-        <v>-77.0229447208942</v>
-      </c>
-      <c r="R26" t="inlineStr">
-        <is>
-          <t>8TH STREET NW AND N STREET NW</t>
-        </is>
-      </c>
       <c r="S26" t="inlineStr">
         <is>
           <t>leon david morton</t>
@@ -2504,7 +2493,7 @@
       </c>
       <c r="T26" t="inlineStr">
         <is>
-          <t>unknown</t>
+          <t>firearm</t>
         </is>
       </c>
     </row>
@@ -2527,11 +2516,11 @@
         </is>
       </c>
       <c r="E27" t="n">
-        <v>100016342</v>
+        <v>100010846</v>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>100016342:1:0</t>
+          <t>100010846:0:0</t>
         </is>
       </c>
       <c r="G27" t="n">
@@ -2564,21 +2553,27 @@
         </is>
       </c>
       <c r="N27" t="n">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="O27" t="inlineStr">
         <is>
           <t>male</t>
         </is>
       </c>
-      <c r="S27" t="inlineStr">
-        <is>
-          <t>leon david morton</t>
+      <c r="P27" t="n">
+        <v>38.9056454536728</v>
+      </c>
+      <c r="Q27" t="n">
+        <v>-77.02399247492311</v>
+      </c>
+      <c r="R27" t="inlineStr">
+        <is>
+          <t>9TH STREET NW AND M STREET NW</t>
         </is>
       </c>
       <c r="T27" t="inlineStr">
         <is>
-          <t>firearm</t>
+          <t>unknown</t>
         </is>
       </c>
     </row>
@@ -2601,11 +2596,11 @@
         </is>
       </c>
       <c r="E28" t="n">
-        <v>100010846</v>
+        <v>100015333</v>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>100010846:0:0</t>
+          <t>100015333:1:0</t>
         </is>
       </c>
       <c r="G28" t="n">
@@ -2638,7 +2633,7 @@
         </is>
       </c>
       <c r="N28" t="n">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O28" t="inlineStr">
         <is>
@@ -2646,14 +2641,19 @@
         </is>
       </c>
       <c r="P28" t="n">
-        <v>38.9056454536728</v>
+        <v>38.9072362908274</v>
       </c>
       <c r="Q28" t="n">
-        <v>-77.02399247492311</v>
+        <v>-77.0229447208942</v>
       </c>
       <c r="R28" t="inlineStr">
         <is>
-          <t>9TH STREET NW AND M STREET NW</t>
+          <t>8TH STREET NW AND N STREET NW</t>
+        </is>
+      </c>
+      <c r="S28" t="inlineStr">
+        <is>
+          <t>leon david morton</t>
         </is>
       </c>
       <c r="T28" t="inlineStr">
@@ -3064,7 +3064,7 @@
         </is>
       </c>
       <c r="C34" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D34" t="inlineStr">
         <is>
@@ -3144,7 +3144,7 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D35" t="inlineStr">
         <is>
@@ -3207,7 +3207,7 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D36" t="inlineStr">
         <is>
@@ -3215,25 +3215,22 @@
         </is>
       </c>
       <c r="E36" t="n">
-        <v>100004364</v>
+        <v>100018683</v>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>100004364:0:0</t>
+          <t>100018683:0:0</t>
         </is>
       </c>
       <c r="G36" t="n">
         <v>2</v>
       </c>
-      <c r="H36" s="3" t="n">
-        <v>28257</v>
-      </c>
       <c r="I36" t="n">
-        <v>2688</v>
+        <v>2692</v>
       </c>
       <c r="J36" t="inlineStr">
         <is>
-          <t>day</t>
+          <t>month</t>
         </is>
       </c>
       <c r="K36" t="inlineStr">
@@ -3251,28 +3248,14 @@
           <t>goodarzi</t>
         </is>
       </c>
-      <c r="N36" t="n">
-        <v>36</v>
-      </c>
-      <c r="O36" t="inlineStr">
-        <is>
-          <t>male</t>
-        </is>
-      </c>
-      <c r="P36" t="n">
-        <v>38.90917468</v>
-      </c>
-      <c r="Q36" t="n">
-        <v>-77.08658868000001</v>
-      </c>
       <c r="R36" t="inlineStr">
         <is>
-          <t>4545 MACARTHUR BOULEVARD NW</t>
+          <t>Rotunda Restaurant, Capitol Hill</t>
         </is>
       </c>
       <c r="T36" t="inlineStr">
         <is>
-          <t>handgun</t>
+          <t>unknown</t>
         </is>
       </c>
     </row>
@@ -3287,7 +3270,7 @@
         </is>
       </c>
       <c r="C37" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D37" t="inlineStr">
         <is>
@@ -3295,22 +3278,25 @@
         </is>
       </c>
       <c r="E37" t="n">
-        <v>100018683</v>
+        <v>100002194</v>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>100018683:0:0</t>
+          <t>100002194:0:0</t>
         </is>
       </c>
       <c r="G37" t="n">
         <v>2</v>
+      </c>
+      <c r="H37" s="3" t="n">
+        <v>28261</v>
       </c>
       <c r="I37" t="n">
         <v>2692</v>
       </c>
       <c r="J37" t="inlineStr">
         <is>
-          <t>month</t>
+          <t>day</t>
         </is>
       </c>
       <c r="K37" t="inlineStr">
@@ -3328,14 +3314,19 @@
           <t>goodarzi</t>
         </is>
       </c>
+      <c r="O37" t="inlineStr">
+        <is>
+          <t>male</t>
+        </is>
+      </c>
       <c r="R37" t="inlineStr">
         <is>
-          <t>Rotunda Restaurant, Capitol Hill</t>
+          <t>Rotunda restaurant</t>
         </is>
       </c>
       <c r="T37" t="inlineStr">
         <is>
-          <t>unknown</t>
+          <t>firearm</t>
         </is>
       </c>
     </row>
@@ -3350,7 +3341,7 @@
         </is>
       </c>
       <c r="C38" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D38" t="inlineStr">
         <is>
@@ -3358,21 +3349,21 @@
         </is>
       </c>
       <c r="E38" t="n">
-        <v>100002194</v>
+        <v>100004364</v>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>100002194:0:0</t>
+          <t>100004364:0:0</t>
         </is>
       </c>
       <c r="G38" t="n">
         <v>2</v>
       </c>
       <c r="H38" s="3" t="n">
-        <v>28261</v>
+        <v>28257</v>
       </c>
       <c r="I38" t="n">
-        <v>2692</v>
+        <v>2688</v>
       </c>
       <c r="J38" t="inlineStr">
         <is>
@@ -3394,19 +3385,28 @@
           <t>goodarzi</t>
         </is>
       </c>
+      <c r="N38" t="n">
+        <v>36</v>
+      </c>
       <c r="O38" t="inlineStr">
         <is>
           <t>male</t>
         </is>
       </c>
+      <c r="P38" t="n">
+        <v>38.90917468</v>
+      </c>
+      <c r="Q38" t="n">
+        <v>-77.08658868000001</v>
+      </c>
       <c r="R38" t="inlineStr">
         <is>
-          <t>Rotunda restaurant</t>
+          <t>4545 MACARTHUR BOULEVARD NW</t>
         </is>
       </c>
       <c r="T38" t="inlineStr">
         <is>
-          <t>firearm</t>
+          <t>handgun</t>
         </is>
       </c>
     </row>
@@ -3421,7 +3421,7 @@
         </is>
       </c>
       <c r="C39" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D39" t="inlineStr">
         <is>
@@ -3429,64 +3429,48 @@
         </is>
       </c>
       <c r="E39" t="n">
-        <v>100001384</v>
+        <v>100009541</v>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>100001384:0:0</t>
+          <t>100009541:0:0</t>
         </is>
       </c>
       <c r="G39" t="n">
         <v>2</v>
       </c>
-      <c r="H39" s="3" t="n">
-        <v>28257</v>
-      </c>
       <c r="I39" t="n">
-        <v>2688</v>
+        <v>2692</v>
       </c>
       <c r="J39" t="inlineStr">
         <is>
-          <t>day</t>
+          <t>month</t>
         </is>
       </c>
       <c r="K39" t="inlineStr">
         <is>
-          <t>Alexis Ahmad Goodarzinia</t>
-        </is>
-      </c>
-      <c r="L39" t="inlineStr">
-        <is>
-          <t>alexis</t>
+          <t>Goodarzi</t>
         </is>
       </c>
       <c r="M39" t="inlineStr">
         <is>
-          <t>goodarzinia</t>
-        </is>
-      </c>
-      <c r="N39" t="n">
-        <v>36</v>
-      </c>
-      <c r="O39" t="inlineStr">
-        <is>
-          <t>male</t>
+          <t>goodarzi</t>
         </is>
       </c>
       <c r="P39" t="n">
-        <v>38.90881714</v>
+        <v>38.92827605</v>
       </c>
       <c r="Q39" t="n">
-        <v>-77.08671231</v>
+        <v>-76.99219773999999</v>
       </c>
       <c r="R39" t="inlineStr">
         <is>
-          <t>4540 MACARTHUR BOULEVARD NW</t>
+          <t>1001 IRVING STREET NE</t>
         </is>
       </c>
       <c r="T39" t="inlineStr">
         <is>
-          <t>firearm</t>
+          <t>unknown</t>
         </is>
       </c>
     </row>
@@ -3497,33 +3481,33 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>100015854:0:0</t>
+          <t>100001184:0:0</t>
         </is>
       </c>
       <c r="C40" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>green</t>
+          <t>goodarzi</t>
         </is>
       </c>
       <c r="E40" t="n">
-        <v>100015854</v>
+        <v>100001384</v>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>100015854:0:0</t>
+          <t>100001384:0:0</t>
         </is>
       </c>
       <c r="G40" t="n">
         <v>2</v>
       </c>
       <c r="H40" s="3" t="n">
-        <v>28334</v>
+        <v>28257</v>
       </c>
       <c r="I40" t="n">
-        <v>2765</v>
+        <v>2688</v>
       </c>
       <c r="J40" t="inlineStr">
         <is>
@@ -3532,21 +3516,21 @@
       </c>
       <c r="K40" t="inlineStr">
         <is>
-          <t>Ernest Green Jr.</t>
+          <t>Alexis Ahmad Goodarzinia</t>
         </is>
       </c>
       <c r="L40" t="inlineStr">
         <is>
-          <t>ernest</t>
+          <t>alexis</t>
         </is>
       </c>
       <c r="M40" t="inlineStr">
         <is>
-          <t>green</t>
+          <t>goodarzinia</t>
         </is>
       </c>
       <c r="N40" t="n">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="O40" t="inlineStr">
         <is>
@@ -3554,19 +3538,14 @@
         </is>
       </c>
       <c r="P40" t="n">
-        <v>38.91455494</v>
+        <v>38.90881714</v>
       </c>
       <c r="Q40" t="n">
-        <v>-77.02786252999999</v>
+        <v>-77.08671231</v>
       </c>
       <c r="R40" t="inlineStr">
         <is>
-          <t>1809 12TH STREET NW</t>
-        </is>
-      </c>
-      <c r="S40" t="inlineStr">
-        <is>
-          <t>ronald r  garnett</t>
+          <t>4540 MACARTHUR BOULEVARD NW</t>
         </is>
       </c>
       <c r="T40" t="inlineStr">
@@ -3582,7 +3561,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>100033283:0:0</t>
+          <t>100015854:0:0</t>
         </is>
       </c>
       <c r="C41" t="n">
@@ -3590,25 +3569,25 @@
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>harper</t>
+          <t>green</t>
         </is>
       </c>
       <c r="E41" t="n">
-        <v>100033283</v>
+        <v>100015854</v>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>100033283:0:0</t>
+          <t>100015854:0:0</t>
         </is>
       </c>
       <c r="G41" t="n">
         <v>2</v>
       </c>
       <c r="H41" s="3" t="n">
-        <v>28427</v>
+        <v>28334</v>
       </c>
       <c r="I41" t="n">
-        <v>2858</v>
+        <v>2765</v>
       </c>
       <c r="J41" t="inlineStr">
         <is>
@@ -3617,21 +3596,21 @@
       </c>
       <c r="K41" t="inlineStr">
         <is>
-          <t>Raymond Harper</t>
+          <t>Ernest Green Jr.</t>
         </is>
       </c>
       <c r="L41" t="inlineStr">
         <is>
-          <t>raymond</t>
+          <t>ernest</t>
         </is>
       </c>
       <c r="M41" t="inlineStr">
         <is>
-          <t>harper</t>
+          <t>green</t>
         </is>
       </c>
       <c r="N41" t="n">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="O41" t="inlineStr">
         <is>
@@ -3639,19 +3618,19 @@
         </is>
       </c>
       <c r="P41" t="n">
-        <v>38.8801759</v>
+        <v>38.91455494</v>
       </c>
       <c r="Q41" t="n">
-        <v>-76.99641043</v>
+        <v>-77.02786252999999</v>
       </c>
       <c r="R41" t="inlineStr">
         <is>
-          <t>731 7TH STREET SE</t>
+          <t>1809 12TH STREET NW</t>
         </is>
       </c>
       <c r="S41" t="inlineStr">
         <is>
-          <t>johnny simms</t>
+          <t>ronald r  garnett</t>
         </is>
       </c>
       <c r="T41" t="inlineStr">
@@ -3667,7 +3646,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>100034545:0:0</t>
+          <t>100033283:0:0</t>
         </is>
       </c>
       <c r="C42" t="n">
@@ -3675,25 +3654,25 @@
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>harris</t>
+          <t>harper</t>
         </is>
       </c>
       <c r="E42" t="n">
-        <v>100034545</v>
+        <v>100033283</v>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>100034545:0:0</t>
+          <t>100033283:0:0</t>
         </is>
       </c>
       <c r="G42" t="n">
         <v>2</v>
       </c>
       <c r="H42" s="3" t="n">
-        <v>28433</v>
+        <v>28427</v>
       </c>
       <c r="I42" t="n">
-        <v>2864</v>
+        <v>2858</v>
       </c>
       <c r="J42" t="inlineStr">
         <is>
@@ -3702,46 +3681,46 @@
       </c>
       <c r="K42" t="inlineStr">
         <is>
-          <t>Margaret Harris</t>
+          <t>Raymond Harper</t>
         </is>
       </c>
       <c r="L42" t="inlineStr">
         <is>
-          <t>margaret</t>
+          <t>raymond</t>
         </is>
       </c>
       <c r="M42" t="inlineStr">
         <is>
-          <t>harris</t>
+          <t>harper</t>
         </is>
       </c>
       <c r="N42" t="n">
-        <v>57</v>
+        <v>21</v>
       </c>
       <c r="O42" t="inlineStr">
         <is>
-          <t>female</t>
+          <t>male</t>
         </is>
       </c>
       <c r="P42" t="n">
-        <v>38.91532904</v>
+        <v>38.8801759</v>
       </c>
       <c r="Q42" t="n">
-        <v>-77.02926796</v>
+        <v>-76.99641043</v>
       </c>
       <c r="R42" t="inlineStr">
         <is>
-          <t>1839 13TH STREET NW</t>
+          <t>731 7TH STREET SE</t>
         </is>
       </c>
       <c r="S42" t="inlineStr">
         <is>
-          <t>gaston brakes</t>
+          <t>johnny simms</t>
         </is>
       </c>
       <c r="T42" t="inlineStr">
         <is>
-          <t>blunt object</t>
+          <t>firearm</t>
         </is>
       </c>
     </row>
@@ -3752,7 +3731,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>100057078:0:0</t>
+          <t>100034545:0:0</t>
         </is>
       </c>
       <c r="C43" t="n">
@@ -3764,21 +3743,21 @@
         </is>
       </c>
       <c r="E43" t="n">
-        <v>100057078</v>
+        <v>100034545</v>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>100057078:0:0</t>
+          <t>100034545:0:0</t>
         </is>
       </c>
       <c r="G43" t="n">
         <v>2</v>
       </c>
       <c r="H43" s="3" t="n">
-        <v>28158</v>
+        <v>28433</v>
       </c>
       <c r="I43" t="n">
-        <v>2589</v>
+        <v>2864</v>
       </c>
       <c r="J43" t="inlineStr">
         <is>
@@ -3787,12 +3766,12 @@
       </c>
       <c r="K43" t="inlineStr">
         <is>
-          <t>Pearl Edith Harris</t>
+          <t>Margaret Harris</t>
         </is>
       </c>
       <c r="L43" t="inlineStr">
         <is>
-          <t>pearl</t>
+          <t>margaret</t>
         </is>
       </c>
       <c r="M43" t="inlineStr">
@@ -3801,7 +3780,7 @@
         </is>
       </c>
       <c r="N43" t="n">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="O43" t="inlineStr">
         <is>
@@ -3809,24 +3788,24 @@
         </is>
       </c>
       <c r="P43" t="n">
-        <v>38.93249976</v>
+        <v>38.91532904</v>
       </c>
       <c r="Q43" t="n">
-        <v>-76.987799</v>
+        <v>-77.02926796</v>
       </c>
       <c r="R43" t="inlineStr">
         <is>
-          <t>1327 MONROE STREET NE</t>
+          <t>1839 13TH STREET NW</t>
         </is>
       </c>
       <c r="S43" t="inlineStr">
         <is>
-          <t>charles b  payne</t>
+          <t>gaston brakes</t>
         </is>
       </c>
       <c r="T43" t="inlineStr">
         <is>
-          <t>firearm</t>
+          <t>blunt object</t>
         </is>
       </c>
     </row>
@@ -3837,7 +3816,7 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>100014753:0:0</t>
+          <t>100057078:0:0</t>
         </is>
       </c>
       <c r="C44" t="n">
@@ -3845,25 +3824,25 @@
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>harrison</t>
+          <t>harris</t>
         </is>
       </c>
       <c r="E44" t="n">
-        <v>100014753</v>
+        <v>100057078</v>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>100014753:0:0</t>
+          <t>100057078:0:0</t>
         </is>
       </c>
       <c r="G44" t="n">
         <v>2</v>
       </c>
       <c r="H44" s="3" t="n">
-        <v>28329</v>
+        <v>28158</v>
       </c>
       <c r="I44" t="n">
-        <v>2760</v>
+        <v>2589</v>
       </c>
       <c r="J44" t="inlineStr">
         <is>
@@ -3872,21 +3851,21 @@
       </c>
       <c r="K44" t="inlineStr">
         <is>
-          <t>Annie Belle Harrison</t>
+          <t>Pearl Edith Harris</t>
         </is>
       </c>
       <c r="L44" t="inlineStr">
         <is>
-          <t>annie</t>
+          <t>pearl</t>
         </is>
       </c>
       <c r="M44" t="inlineStr">
         <is>
-          <t>harrison</t>
+          <t>harris</t>
         </is>
       </c>
       <c r="N44" t="n">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="O44" t="inlineStr">
         <is>
@@ -3894,24 +3873,24 @@
         </is>
       </c>
       <c r="P44" t="n">
-        <v>38.9029655833041</v>
+        <v>38.93249976</v>
       </c>
       <c r="Q44" t="n">
-        <v>-76.97873144433829</v>
+        <v>-76.987799</v>
       </c>
       <c r="R44" t="inlineStr">
         <is>
-          <t>1013 17TH STREET NE</t>
+          <t>1327 MONROE STREET NE</t>
         </is>
       </c>
       <c r="S44" t="inlineStr">
         <is>
-          <t>norman b  brown</t>
+          <t>charles b  payne</t>
         </is>
       </c>
       <c r="T44" t="inlineStr">
         <is>
-          <t>knife</t>
+          <t>firearm</t>
         </is>
       </c>
     </row>
@@ -3922,7 +3901,7 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>100042269:0:0</t>
+          <t>100014753:0:0</t>
         </is>
       </c>
       <c r="C45" t="n">
@@ -3930,25 +3909,25 @@
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>hicks</t>
+          <t>harrison</t>
         </is>
       </c>
       <c r="E45" t="n">
-        <v>100042269</v>
+        <v>100014753</v>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>100042269:0:0</t>
+          <t>100014753:0:0</t>
         </is>
       </c>
       <c r="G45" t="n">
         <v>2</v>
       </c>
       <c r="H45" s="3" t="n">
-        <v>28472</v>
+        <v>28329</v>
       </c>
       <c r="I45" t="n">
-        <v>2903</v>
+        <v>2760</v>
       </c>
       <c r="J45" t="inlineStr">
         <is>
@@ -3957,21 +3936,21 @@
       </c>
       <c r="K45" t="inlineStr">
         <is>
-          <t>Jacqueline Hicks</t>
+          <t>Annie Belle Harrison</t>
         </is>
       </c>
       <c r="L45" t="inlineStr">
         <is>
-          <t>jacqueline</t>
+          <t>annie</t>
         </is>
       </c>
       <c r="M45" t="inlineStr">
         <is>
-          <t>hicks</t>
+          <t>harrison</t>
         </is>
       </c>
       <c r="N45" t="n">
-        <v>20</v>
+        <v>69</v>
       </c>
       <c r="O45" t="inlineStr">
         <is>
@@ -3979,19 +3958,24 @@
         </is>
       </c>
       <c r="P45" t="n">
-        <v>38.90319026</v>
+        <v>38.9029655833041</v>
       </c>
       <c r="Q45" t="n">
-        <v>-76.97243071</v>
+        <v>-76.97873144433829</v>
       </c>
       <c r="R45" t="inlineStr">
         <is>
-          <t>2121 I STREET NE</t>
+          <t>1013 17TH STREET NE</t>
+        </is>
+      </c>
+      <c r="S45" t="inlineStr">
+        <is>
+          <t>norman b  brown</t>
         </is>
       </c>
       <c r="T45" t="inlineStr">
         <is>
-          <t>firearm</t>
+          <t>knife</t>
         </is>
       </c>
     </row>
@@ -4002,7 +3986,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>100044573:0:0</t>
+          <t>100042269:0:0</t>
         </is>
       </c>
       <c r="C46" t="n">
@@ -4010,25 +3994,25 @@
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>hughes</t>
+          <t>hicks</t>
         </is>
       </c>
       <c r="E46" t="n">
-        <v>100044573</v>
+        <v>100042269</v>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>100044573:0:0</t>
+          <t>100042269:0:0</t>
         </is>
       </c>
       <c r="G46" t="n">
         <v>2</v>
       </c>
       <c r="H46" s="3" t="n">
-        <v>28483</v>
+        <v>28472</v>
       </c>
       <c r="I46" t="n">
-        <v>2914</v>
+        <v>2903</v>
       </c>
       <c r="J46" t="inlineStr">
         <is>
@@ -4037,41 +4021,36 @@
       </c>
       <c r="K46" t="inlineStr">
         <is>
-          <t>Wendell Ernest Hughes</t>
+          <t>Jacqueline Hicks</t>
         </is>
       </c>
       <c r="L46" t="inlineStr">
         <is>
-          <t>wendell</t>
+          <t>jacqueline</t>
         </is>
       </c>
       <c r="M46" t="inlineStr">
         <is>
-          <t>hughes</t>
+          <t>hicks</t>
         </is>
       </c>
       <c r="N46" t="n">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="O46" t="inlineStr">
         <is>
-          <t>male</t>
+          <t>female</t>
         </is>
       </c>
       <c r="P46" t="n">
-        <v>38.9203932</v>
+        <v>38.90319026</v>
       </c>
       <c r="Q46" t="n">
-        <v>-77.00221635</v>
+        <v>-76.97243071</v>
       </c>
       <c r="R46" t="inlineStr">
         <is>
-          <t>234 ADAMS STREET NE</t>
-        </is>
-      </c>
-      <c r="S46" t="inlineStr">
-        <is>
-          <t>james jackson</t>
+          <t>2121 I STREET NE</t>
         </is>
       </c>
       <c r="T46" t="inlineStr">
@@ -4087,7 +4066,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>100068635:0:0</t>
+          <t>100044573:0:0</t>
         </is>
       </c>
       <c r="C47" t="n">
@@ -4095,25 +4074,25 @@
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>jackson</t>
+          <t>hughes</t>
         </is>
       </c>
       <c r="E47" t="n">
-        <v>100068635</v>
+        <v>100044573</v>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>100068635:0:0</t>
+          <t>100044573:0:0</t>
         </is>
       </c>
       <c r="G47" t="n">
         <v>2</v>
       </c>
       <c r="H47" s="3" t="n">
-        <v>28249</v>
+        <v>28483</v>
       </c>
       <c r="I47" t="n">
-        <v>2680</v>
+        <v>2914</v>
       </c>
       <c r="J47" t="inlineStr">
         <is>
@@ -4122,21 +4101,21 @@
       </c>
       <c r="K47" t="inlineStr">
         <is>
-          <t>James E. Jackson</t>
+          <t>Wendell Ernest Hughes</t>
         </is>
       </c>
       <c r="L47" t="inlineStr">
         <is>
-          <t>james</t>
+          <t>wendell</t>
         </is>
       </c>
       <c r="M47" t="inlineStr">
         <is>
-          <t>jackson</t>
+          <t>hughes</t>
         </is>
       </c>
       <c r="N47" t="n">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="O47" t="inlineStr">
         <is>
@@ -4144,14 +4123,19 @@
         </is>
       </c>
       <c r="P47" t="n">
-        <v>38.9003934655188</v>
+        <v>38.9203932</v>
       </c>
       <c r="Q47" t="n">
-        <v>-76.99525762115221</v>
+        <v>-77.00221635</v>
       </c>
       <c r="R47" t="inlineStr">
         <is>
-          <t>720 H STREET NE</t>
+          <t>234 ADAMS STREET NE</t>
+        </is>
+      </c>
+      <c r="S47" t="inlineStr">
+        <is>
+          <t>james jackson</t>
         </is>
       </c>
       <c r="T47" t="inlineStr">
@@ -4167,7 +4151,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>100016685:0:0</t>
+          <t>100068635:0:0</t>
         </is>
       </c>
       <c r="C48" t="n">
@@ -4179,21 +4163,21 @@
         </is>
       </c>
       <c r="E48" t="n">
-        <v>100016685</v>
+        <v>100068635</v>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>100016685:0:0</t>
+          <t>100068635:0:0</t>
         </is>
       </c>
       <c r="G48" t="n">
         <v>2</v>
       </c>
       <c r="H48" s="3" t="n">
-        <v>28339</v>
+        <v>28249</v>
       </c>
       <c r="I48" t="n">
-        <v>2770</v>
+        <v>2680</v>
       </c>
       <c r="J48" t="inlineStr">
         <is>
@@ -4202,12 +4186,12 @@
       </c>
       <c r="K48" t="inlineStr">
         <is>
-          <t>John Jackson</t>
+          <t>James E. Jackson</t>
         </is>
       </c>
       <c r="L48" t="inlineStr">
         <is>
-          <t>john</t>
+          <t>james</t>
         </is>
       </c>
       <c r="M48" t="inlineStr">
@@ -4216,7 +4200,7 @@
         </is>
       </c>
       <c r="N48" t="n">
-        <v>65</v>
+        <v>22</v>
       </c>
       <c r="O48" t="inlineStr">
         <is>
@@ -4224,24 +4208,19 @@
         </is>
       </c>
       <c r="P48" t="n">
-        <v>38.94423014</v>
+        <v>38.9003934655188</v>
       </c>
       <c r="Q48" t="n">
-        <v>-77.02366465</v>
+        <v>-76.99525762115221</v>
       </c>
       <c r="R48" t="inlineStr">
         <is>
-          <t>801 WEBSTER STREET NW</t>
-        </is>
-      </c>
-      <c r="S48" t="inlineStr">
-        <is>
-          <t>gleana long</t>
+          <t>720 H STREET NE</t>
         </is>
       </c>
       <c r="T48" t="inlineStr">
         <is>
-          <t>knife</t>
+          <t>firearm</t>
         </is>
       </c>
     </row>
@@ -4252,7 +4231,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>100063507:0:0</t>
+          <t>100016685:0:0</t>
         </is>
       </c>
       <c r="C49" t="n">
@@ -4260,25 +4239,25 @@
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>james</t>
+          <t>jackson</t>
         </is>
       </c>
       <c r="E49" t="n">
-        <v>100063507</v>
+        <v>100016685</v>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>100063507:0:0</t>
+          <t>100016685:0:0</t>
         </is>
       </c>
       <c r="G49" t="n">
         <v>2</v>
       </c>
       <c r="H49" s="3" t="n">
-        <v>28219</v>
+        <v>28339</v>
       </c>
       <c r="I49" t="n">
-        <v>2650</v>
+        <v>2770</v>
       </c>
       <c r="J49" t="inlineStr">
         <is>
@@ -4287,21 +4266,21 @@
       </c>
       <c r="K49" t="inlineStr">
         <is>
-          <t>Willy James</t>
+          <t>John Jackson</t>
         </is>
       </c>
       <c r="L49" t="inlineStr">
         <is>
-          <t>willy</t>
+          <t>john</t>
         </is>
       </c>
       <c r="M49" t="inlineStr">
         <is>
-          <t>james</t>
+          <t>jackson</t>
         </is>
       </c>
       <c r="N49" t="n">
-        <v>46</v>
+        <v>65</v>
       </c>
       <c r="O49" t="inlineStr">
         <is>
@@ -4309,19 +4288,24 @@
         </is>
       </c>
       <c r="P49" t="n">
-        <v>38.90151736</v>
+        <v>38.94423014</v>
       </c>
       <c r="Q49" t="n">
-        <v>-76.99247816</v>
+        <v>-77.02366465</v>
       </c>
       <c r="R49" t="inlineStr">
         <is>
-          <t>1000 I STREET NE</t>
+          <t>801 WEBSTER STREET NW</t>
+        </is>
+      </c>
+      <c r="S49" t="inlineStr">
+        <is>
+          <t>gleana long</t>
         </is>
       </c>
       <c r="T49" t="inlineStr">
         <is>
-          <t>firearm</t>
+          <t>knife</t>
         </is>
       </c>
     </row>
@@ -4332,7 +4316,7 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>100004722:0:0</t>
+          <t>100063507:0:0</t>
         </is>
       </c>
       <c r="C50" t="n">
@@ -4340,25 +4324,25 @@
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>jeffries</t>
+          <t>james</t>
         </is>
       </c>
       <c r="E50" t="n">
-        <v>100004722</v>
+        <v>100063507</v>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>100004722:0:0</t>
+          <t>100063507:0:0</t>
         </is>
       </c>
       <c r="G50" t="n">
         <v>2</v>
       </c>
       <c r="H50" s="3" t="n">
-        <v>28275</v>
+        <v>28219</v>
       </c>
       <c r="I50" t="n">
-        <v>2706</v>
+        <v>2650</v>
       </c>
       <c r="J50" t="inlineStr">
         <is>
@@ -4367,21 +4351,21 @@
       </c>
       <c r="K50" t="inlineStr">
         <is>
-          <t>Joe L. Jeffries</t>
+          <t>Willy James</t>
         </is>
       </c>
       <c r="L50" t="inlineStr">
         <is>
-          <t>joe</t>
+          <t>willy</t>
         </is>
       </c>
       <c r="M50" t="inlineStr">
         <is>
-          <t>jeffries</t>
+          <t>james</t>
         </is>
       </c>
       <c r="N50" t="n">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="O50" t="inlineStr">
         <is>
@@ -4389,24 +4373,19 @@
         </is>
       </c>
       <c r="P50" t="n">
-        <v>38.90233267</v>
+        <v>38.90151736</v>
       </c>
       <c r="Q50" t="n">
-        <v>-76.97483185999999</v>
+        <v>-76.99247816</v>
       </c>
       <c r="R50" t="inlineStr">
         <is>
-          <t>2005 I STREET NE</t>
-        </is>
-      </c>
-      <c r="S50" t="inlineStr">
-        <is>
-          <t>timothy b  wilson</t>
+          <t>1000 I STREET NE</t>
         </is>
       </c>
       <c r="T50" t="inlineStr">
         <is>
-          <t>handgun</t>
+          <t>firearm</t>
         </is>
       </c>
     </row>
@@ -4417,7 +4396,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>100063971:0:0</t>
+          <t>100004722:0:0</t>
         </is>
       </c>
       <c r="C51" t="n">
@@ -4425,25 +4404,25 @@
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>johnson</t>
+          <t>jeffries</t>
         </is>
       </c>
       <c r="E51" t="n">
-        <v>100063971</v>
+        <v>100004722</v>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>100063971:0:0</t>
+          <t>100004722:0:0</t>
         </is>
       </c>
       <c r="G51" t="n">
         <v>2</v>
       </c>
       <c r="H51" s="3" t="n">
-        <v>28205</v>
+        <v>28275</v>
       </c>
       <c r="I51" t="n">
-        <v>2636</v>
+        <v>2706</v>
       </c>
       <c r="J51" t="inlineStr">
         <is>
@@ -4452,21 +4431,21 @@
       </c>
       <c r="K51" t="inlineStr">
         <is>
-          <t>David Lee Johnson</t>
+          <t>Joe L. Jeffries</t>
         </is>
       </c>
       <c r="L51" t="inlineStr">
         <is>
-          <t>david</t>
+          <t>joe</t>
         </is>
       </c>
       <c r="M51" t="inlineStr">
         <is>
-          <t>johnson</t>
+          <t>jeffries</t>
         </is>
       </c>
       <c r="N51" t="n">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="O51" t="inlineStr">
         <is>
@@ -4474,24 +4453,24 @@
         </is>
       </c>
       <c r="P51" t="n">
-        <v>38.9019175186715</v>
+        <v>38.90233267</v>
       </c>
       <c r="Q51" t="n">
-        <v>-76.99375420307049</v>
+        <v>-76.97483185999999</v>
       </c>
       <c r="R51" t="inlineStr">
         <is>
-          <t>9TH STREET NE FROM I STREET NE TO K STREET NE</t>
+          <t>2005 I STREET NE</t>
         </is>
       </c>
       <c r="S51" t="inlineStr">
         <is>
-          <t>michael stanley davis</t>
+          <t>timothy b  wilson</t>
         </is>
       </c>
       <c r="T51" t="inlineStr">
         <is>
-          <t>firearm</t>
+          <t>handgun</t>
         </is>
       </c>
     </row>
@@ -4502,7 +4481,7 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>100044008:0:0</t>
+          <t>100063971:0:0</t>
         </is>
       </c>
       <c r="C52" t="n">
@@ -4514,21 +4493,21 @@
         </is>
       </c>
       <c r="E52" t="n">
-        <v>100044008</v>
+        <v>100063971</v>
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>100044008:0:0</t>
+          <t>100063971:0:0</t>
         </is>
       </c>
       <c r="G52" t="n">
         <v>2</v>
       </c>
       <c r="H52" s="3" t="n">
-        <v>28479</v>
+        <v>28205</v>
       </c>
       <c r="I52" t="n">
-        <v>2910</v>
+        <v>2636</v>
       </c>
       <c r="J52" t="inlineStr">
         <is>
@@ -4537,12 +4516,12 @@
       </c>
       <c r="K52" t="inlineStr">
         <is>
-          <t>William C. Johnson</t>
+          <t>David Lee Johnson</t>
         </is>
       </c>
       <c r="L52" t="inlineStr">
         <is>
-          <t>william</t>
+          <t>david</t>
         </is>
       </c>
       <c r="M52" t="inlineStr">
@@ -4551,7 +4530,7 @@
         </is>
       </c>
       <c r="N52" t="n">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="O52" t="inlineStr">
         <is>
@@ -4559,19 +4538,19 @@
         </is>
       </c>
       <c r="P52" t="n">
-        <v>38.8813219299484</v>
+        <v>38.9019175186715</v>
       </c>
       <c r="Q52" t="n">
-        <v>-76.9268837050888</v>
+        <v>-76.99375420307049</v>
       </c>
       <c r="R52" t="inlineStr">
         <is>
-          <t>53RD STREET SE AND F STREET SE</t>
+          <t>9TH STREET NE FROM I STREET NE TO K STREET NE</t>
         </is>
       </c>
       <c r="S52" t="inlineStr">
         <is>
-          <t>michael a  short</t>
+          <t>michael stanley davis</t>
         </is>
       </c>
       <c r="T52" t="inlineStr">
@@ -4587,7 +4566,7 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>100022057:0:0</t>
+          <t>100044008:0:0</t>
         </is>
       </c>
       <c r="C53" t="n">
@@ -4595,25 +4574,25 @@
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>jones</t>
+          <t>johnson</t>
         </is>
       </c>
       <c r="E53" t="n">
-        <v>100022057</v>
+        <v>100044008</v>
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>100022057:0:0</t>
+          <t>100044008:0:0</t>
         </is>
       </c>
       <c r="G53" t="n">
         <v>2</v>
       </c>
       <c r="H53" s="3" t="n">
-        <v>28369</v>
+        <v>28479</v>
       </c>
       <c r="I53" t="n">
-        <v>2800</v>
+        <v>2910</v>
       </c>
       <c r="J53" t="inlineStr">
         <is>
@@ -4622,21 +4601,21 @@
       </c>
       <c r="K53" t="inlineStr">
         <is>
-          <t>Andrew V. Jones</t>
+          <t>William C. Johnson</t>
         </is>
       </c>
       <c r="L53" t="inlineStr">
         <is>
-          <t>andrew</t>
+          <t>william</t>
         </is>
       </c>
       <c r="M53" t="inlineStr">
         <is>
-          <t>jones</t>
+          <t>johnson</t>
         </is>
       </c>
       <c r="N53" t="n">
-        <v>28</v>
+        <v>56</v>
       </c>
       <c r="O53" t="inlineStr">
         <is>
@@ -4644,14 +4623,19 @@
         </is>
       </c>
       <c r="P53" t="n">
-        <v>38.9025143016862</v>
+        <v>38.8813219299484</v>
       </c>
       <c r="Q53" t="n">
-        <v>-77.0013046915693</v>
+        <v>-76.9268837050888</v>
       </c>
       <c r="R53" t="inlineStr">
         <is>
-          <t>K STREET NE FROM 3RD STREET NE TO 4TH STREET NE</t>
+          <t>53RD STREET SE AND F STREET SE</t>
+        </is>
+      </c>
+      <c r="S53" t="inlineStr">
+        <is>
+          <t>michael a  short</t>
         </is>
       </c>
       <c r="T53" t="inlineStr">
@@ -4667,11 +4651,11 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>100020589:0:0</t>
+          <t>100022057:0:0</t>
         </is>
       </c>
       <c r="C54" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D54" t="inlineStr">
         <is>
@@ -4679,21 +4663,21 @@
         </is>
       </c>
       <c r="E54" t="n">
-        <v>100021528</v>
+        <v>100022057</v>
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>100021528:0:0</t>
+          <t>100022057:0:0</t>
         </is>
       </c>
       <c r="G54" t="n">
         <v>2</v>
       </c>
       <c r="H54" s="3" t="n">
-        <v>28360</v>
+        <v>28369</v>
       </c>
       <c r="I54" t="n">
-        <v>2791</v>
+        <v>2800</v>
       </c>
       <c r="J54" t="inlineStr">
         <is>
@@ -4702,12 +4686,12 @@
       </c>
       <c r="K54" t="inlineStr">
         <is>
-          <t>Perry Jones, Jr.</t>
+          <t>Andrew V. Jones</t>
         </is>
       </c>
       <c r="L54" t="inlineStr">
         <is>
-          <t>perry</t>
+          <t>andrew</t>
         </is>
       </c>
       <c r="M54" t="inlineStr">
@@ -4716,7 +4700,7 @@
         </is>
       </c>
       <c r="N54" t="n">
-        <v>57</v>
+        <v>28</v>
       </c>
       <c r="O54" t="inlineStr">
         <is>
@@ -4724,14 +4708,14 @@
         </is>
       </c>
       <c r="P54" t="n">
-        <v>38.90486457</v>
+        <v>38.9025143016862</v>
       </c>
       <c r="Q54" t="n">
-        <v>-77.04700411</v>
+        <v>-77.0013046915693</v>
       </c>
       <c r="R54" t="inlineStr">
         <is>
-          <t>2100 M STREET NW</t>
+          <t>K STREET NE FROM 3RD STREET NE TO 4TH STREET NE</t>
         </is>
       </c>
       <c r="T54" t="inlineStr">
@@ -4759,11 +4743,11 @@
         </is>
       </c>
       <c r="E55" t="n">
-        <v>100020589</v>
+        <v>100021528</v>
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>100020589:0:0</t>
+          <t>100021528:0:0</t>
         </is>
       </c>
       <c r="G55" t="n">
@@ -4782,12 +4766,12 @@
       </c>
       <c r="K55" t="inlineStr">
         <is>
-          <t>Terry Jones</t>
+          <t>Perry Jones, Jr.</t>
         </is>
       </c>
       <c r="L55" t="inlineStr">
         <is>
-          <t>terry</t>
+          <t>perry</t>
         </is>
       </c>
       <c r="M55" t="inlineStr">
@@ -4796,7 +4780,7 @@
         </is>
       </c>
       <c r="N55" t="n">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="O55" t="inlineStr">
         <is>
@@ -4804,14 +4788,14 @@
         </is>
       </c>
       <c r="P55" t="n">
-        <v>38.9245292320447</v>
+        <v>38.90486457</v>
       </c>
       <c r="Q55" t="n">
-        <v>-77.0304740748672</v>
+        <v>-77.04700411</v>
       </c>
       <c r="R55" t="inlineStr">
         <is>
-          <t>1316 FAIRMONT STREET NW</t>
+          <t>2100 M STREET NW</t>
         </is>
       </c>
       <c r="T55" t="inlineStr">
@@ -4827,11 +4811,11 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>100026182:0:0</t>
+          <t>100020589:0:0</t>
         </is>
       </c>
       <c r="C56" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D56" t="inlineStr">
         <is>
@@ -4839,21 +4823,21 @@
         </is>
       </c>
       <c r="E56" t="n">
-        <v>100026182</v>
+        <v>100020589</v>
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>100026182:0:0</t>
+          <t>100020589:0:0</t>
         </is>
       </c>
       <c r="G56" t="n">
         <v>2</v>
       </c>
       <c r="H56" s="3" t="n">
-        <v>28382</v>
+        <v>28360</v>
       </c>
       <c r="I56" t="n">
-        <v>2813</v>
+        <v>2791</v>
       </c>
       <c r="J56" t="inlineStr">
         <is>
@@ -4862,12 +4846,12 @@
       </c>
       <c r="K56" t="inlineStr">
         <is>
-          <t>William Jones</t>
+          <t>Terry Jones</t>
         </is>
       </c>
       <c r="L56" t="inlineStr">
         <is>
-          <t>william</t>
+          <t>terry</t>
         </is>
       </c>
       <c r="M56" t="inlineStr">
@@ -4876,7 +4860,7 @@
         </is>
       </c>
       <c r="N56" t="n">
-        <v>37</v>
+        <v>55</v>
       </c>
       <c r="O56" t="inlineStr">
         <is>
@@ -4884,14 +4868,14 @@
         </is>
       </c>
       <c r="P56" t="n">
-        <v>38.85785074</v>
+        <v>38.9245292320447</v>
       </c>
       <c r="Q56" t="n">
-        <v>-76.9873077</v>
+        <v>-77.0304740748672</v>
       </c>
       <c r="R56" t="inlineStr">
         <is>
-          <t>2702 STANTON ROAD SE</t>
+          <t>1316 FAIRMONT STREET NW</t>
         </is>
       </c>
       <c r="T56" t="inlineStr">
@@ -5259,21 +5243,21 @@
         </is>
       </c>
       <c r="E61" t="n">
-        <v>100025319</v>
+        <v>100037322</v>
       </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t>100025319:0:0</t>
+          <t>100037322:0:0</t>
         </is>
       </c>
       <c r="G61" t="n">
         <v>2</v>
       </c>
       <c r="H61" s="3" t="n">
-        <v>28381</v>
+        <v>28378</v>
       </c>
       <c r="I61" t="n">
-        <v>2812</v>
+        <v>2809</v>
       </c>
       <c r="J61" t="inlineStr">
         <is>
@@ -5282,7 +5266,7 @@
       </c>
       <c r="K61" t="inlineStr">
         <is>
-          <t>Vernon McKinley</t>
+          <t>Vernon McKinely</t>
         </is>
       </c>
       <c r="L61" t="inlineStr">
@@ -5292,7 +5276,7 @@
       </c>
       <c r="M61" t="inlineStr">
         <is>
-          <t>mckinley</t>
+          <t>mckinely</t>
         </is>
       </c>
       <c r="N61" t="n">
@@ -5314,9 +5298,14 @@
           <t>709 ANACOSTIA AVENUE NE</t>
         </is>
       </c>
+      <c r="S61" t="inlineStr">
+        <is>
+          <t>joseph west</t>
+        </is>
+      </c>
       <c r="T61" t="inlineStr">
         <is>
-          <t>unknown</t>
+          <t>handgun</t>
         </is>
       </c>
     </row>
@@ -5339,21 +5328,21 @@
         </is>
       </c>
       <c r="E62" t="n">
-        <v>100037322</v>
+        <v>100025319</v>
       </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t>100037322:0:0</t>
+          <t>100025319:0:0</t>
         </is>
       </c>
       <c r="G62" t="n">
         <v>2</v>
       </c>
       <c r="H62" s="3" t="n">
-        <v>28378</v>
+        <v>28381</v>
       </c>
       <c r="I62" t="n">
-        <v>2809</v>
+        <v>2812</v>
       </c>
       <c r="J62" t="inlineStr">
         <is>
@@ -5384,24 +5373,19 @@
         </is>
       </c>
       <c r="P62" t="n">
-        <v>38.9016962562781</v>
+        <v>38.90163219</v>
       </c>
       <c r="Q62" t="n">
-        <v>-76.9510057422886</v>
+        <v>-76.95075158</v>
       </c>
       <c r="R62" t="inlineStr">
         <is>
-          <t>ANACOSTIA AVENUE NE FROM GRANT PLACE NE TO ALBERT IRVIN CASSELL PLACE NE</t>
-        </is>
-      </c>
-      <c r="S62" t="inlineStr">
-        <is>
-          <t>joseph west</t>
+          <t>709 ANACOSTIA AVENUE NE</t>
         </is>
       </c>
       <c r="T62" t="inlineStr">
         <is>
-          <t>handgun</t>
+          <t>unknown</t>
         </is>
       </c>
     </row>
@@ -6397,22 +6381,25 @@
         </is>
       </c>
       <c r="E75" t="n">
-        <v>100010427</v>
+        <v>100004075</v>
       </c>
       <c r="F75" t="inlineStr">
         <is>
-          <t>100010427:0:0</t>
+          <t>100004075:0:0</t>
         </is>
       </c>
       <c r="G75" t="n">
         <v>2</v>
       </c>
+      <c r="H75" s="3" t="n">
+        <v>28271</v>
+      </c>
       <c r="I75" t="n">
-        <v>2692</v>
+        <v>2702</v>
       </c>
       <c r="J75" t="inlineStr">
         <is>
-          <t>month</t>
+          <t>day</t>
         </is>
       </c>
       <c r="K75" t="inlineStr">
@@ -6430,14 +6417,28 @@
           <t>proctor</t>
         </is>
       </c>
+      <c r="N75" t="n">
+        <v>19</v>
+      </c>
       <c r="O75" t="inlineStr">
         <is>
           <t>male</t>
         </is>
       </c>
+      <c r="P75" t="n">
+        <v>38.92200396</v>
+      </c>
+      <c r="Q75" t="n">
+        <v>-77.03236063</v>
+      </c>
+      <c r="R75" t="inlineStr">
+        <is>
+          <t>2500 14TH STREET NW</t>
+        </is>
+      </c>
       <c r="S75" t="inlineStr">
         <is>
-          <t>john e  fuller</t>
+          <t>john edward fuller</t>
         </is>
       </c>
       <c r="T75" t="inlineStr">
@@ -6465,25 +6466,22 @@
         </is>
       </c>
       <c r="E76" t="n">
-        <v>100004075</v>
+        <v>100010427</v>
       </c>
       <c r="F76" t="inlineStr">
         <is>
-          <t>100004075:0:0</t>
+          <t>100010427:0:0</t>
         </is>
       </c>
       <c r="G76" t="n">
         <v>2</v>
       </c>
-      <c r="H76" s="3" t="n">
-        <v>28271</v>
-      </c>
       <c r="I76" t="n">
-        <v>2702</v>
+        <v>2692</v>
       </c>
       <c r="J76" t="inlineStr">
         <is>
-          <t>day</t>
+          <t>month</t>
         </is>
       </c>
       <c r="K76" t="inlineStr">
@@ -6501,28 +6499,14 @@
           <t>proctor</t>
         </is>
       </c>
-      <c r="N76" t="n">
-        <v>19</v>
-      </c>
       <c r="O76" t="inlineStr">
         <is>
           <t>male</t>
         </is>
       </c>
-      <c r="P76" t="n">
-        <v>38.92200396</v>
-      </c>
-      <c r="Q76" t="n">
-        <v>-77.03236063</v>
-      </c>
-      <c r="R76" t="inlineStr">
-        <is>
-          <t>2500 14TH STREET NW</t>
-        </is>
-      </c>
       <c r="S76" t="inlineStr">
         <is>
-          <t>john edward fuller</t>
+          <t>john e  fuller</t>
         </is>
       </c>
       <c r="T76" t="inlineStr">
@@ -7145,25 +7129,22 @@
         </is>
       </c>
       <c r="E84" t="n">
-        <v>100040692</v>
+        <v>100040873</v>
       </c>
       <c r="F84" t="inlineStr">
         <is>
-          <t>100040692:1:0</t>
+          <t>100040873:0:1</t>
         </is>
       </c>
       <c r="G84" t="n">
         <v>2</v>
       </c>
-      <c r="H84" s="3" t="n">
-        <v>28464</v>
-      </c>
       <c r="I84" t="n">
-        <v>2895</v>
+        <v>2906</v>
       </c>
       <c r="J84" t="inlineStr">
         <is>
-          <t>day</t>
+          <t>month</t>
         </is>
       </c>
       <c r="K84" t="inlineStr">
@@ -7189,15 +7170,14 @@
           <t>male</t>
         </is>
       </c>
-      <c r="P84" t="n">
-        <v>38.8841290284262</v>
-      </c>
-      <c r="Q84" t="n">
-        <v>-76.9307169045053</v>
-      </c>
       <c r="R84" t="inlineStr">
         <is>
-          <t>360 50TH STREET SE</t>
+          <t>Fort DuPont Park, SE</t>
+        </is>
+      </c>
+      <c r="S84" t="inlineStr">
+        <is>
+          <t>james m  head</t>
         </is>
       </c>
       <c r="T84" t="inlineStr">
@@ -7225,22 +7205,25 @@
         </is>
       </c>
       <c r="E85" t="n">
-        <v>100040873</v>
+        <v>100040692</v>
       </c>
       <c r="F85" t="inlineStr">
         <is>
-          <t>100040873:0:1</t>
+          <t>100040692:1:0</t>
         </is>
       </c>
       <c r="G85" t="n">
         <v>2</v>
       </c>
+      <c r="H85" s="3" t="n">
+        <v>28464</v>
+      </c>
       <c r="I85" t="n">
-        <v>2906</v>
+        <v>2895</v>
       </c>
       <c r="J85" t="inlineStr">
         <is>
-          <t>month</t>
+          <t>day</t>
         </is>
       </c>
       <c r="K85" t="inlineStr">
@@ -7266,14 +7249,15 @@
           <t>male</t>
         </is>
       </c>
+      <c r="P85" t="n">
+        <v>38.8841290284262</v>
+      </c>
+      <c r="Q85" t="n">
+        <v>-76.9307169045053</v>
+      </c>
       <c r="R85" t="inlineStr">
         <is>
-          <t>Fort DuPont Park, SE</t>
-        </is>
-      </c>
-      <c r="S85" t="inlineStr">
-        <is>
-          <t>james m  head</t>
+          <t>360 50TH STREET SE</t>
         </is>
       </c>
       <c r="T85" t="inlineStr">
@@ -7536,70 +7520,78 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>100025447:0:0</t>
+          <t>100054861:0:0</t>
         </is>
       </c>
       <c r="C89" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>taylor</t>
+          <t>watson</t>
         </is>
       </c>
       <c r="E89" t="n">
-        <v>100025447</v>
+        <v>100056154</v>
       </c>
       <c r="F89" t="inlineStr">
         <is>
-          <t>100025447:0:0</t>
+          <t>100056154:0:0</t>
         </is>
       </c>
       <c r="G89" t="n">
         <v>2</v>
       </c>
-      <c r="H89" s="3" t="n">
-        <v>28381</v>
-      </c>
       <c r="I89" t="n">
-        <v>2812</v>
+        <v>2601</v>
       </c>
       <c r="J89" t="inlineStr">
         <is>
-          <t>day</t>
+          <t>month</t>
         </is>
       </c>
       <c r="K89" t="inlineStr">
         <is>
-          <t>Julian Taylor</t>
+          <t>Arthur Lee Watson</t>
         </is>
       </c>
       <c r="L89" t="inlineStr">
         <is>
-          <t>julian</t>
+          <t>arthur</t>
         </is>
       </c>
       <c r="M89" t="inlineStr">
         <is>
-          <t>taylor</t>
+          <t>watson</t>
         </is>
       </c>
       <c r="N89" t="n">
-        <v>63</v>
+        <v>21</v>
       </c>
       <c r="O89" t="inlineStr">
         <is>
           <t>male</t>
         </is>
       </c>
+      <c r="P89" t="n">
+        <v>38.92200396</v>
+      </c>
+      <c r="Q89" t="n">
+        <v>-77.03236063</v>
+      </c>
       <c r="R89" t="inlineStr">
         <is>
-          <t>Portland St and Martin Luther King Ave SE</t>
+          <t>2500 14TH STREET NW</t>
+        </is>
+      </c>
+      <c r="S89" t="inlineStr">
+        <is>
+          <t>harold mitchell</t>
         </is>
       </c>
       <c r="T89" t="inlineStr">
         <is>
-          <t>handgun</t>
+          <t>firearm</t>
         </is>
       </c>
     </row>
@@ -7695,11 +7687,11 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>100054861:0:0</t>
+          <t>100056434:0:0</t>
         </is>
       </c>
       <c r="C91" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D91" t="inlineStr">
         <is>
@@ -7707,32 +7699,35 @@
         </is>
       </c>
       <c r="E91" t="n">
-        <v>100056154</v>
+        <v>100056434</v>
       </c>
       <c r="F91" t="inlineStr">
         <is>
-          <t>100056154:0:0</t>
+          <t>100056434:0:0</t>
         </is>
       </c>
       <c r="G91" t="n">
         <v>2</v>
       </c>
+      <c r="H91" s="3" t="n">
+        <v>28129</v>
+      </c>
       <c r="I91" t="n">
-        <v>2601</v>
+        <v>2560</v>
       </c>
       <c r="J91" t="inlineStr">
         <is>
-          <t>month</t>
+          <t>day</t>
         </is>
       </c>
       <c r="K91" t="inlineStr">
         <is>
-          <t>Arthur Lee Watson</t>
+          <t>Claibourne Watson</t>
         </is>
       </c>
       <c r="L91" t="inlineStr">
         <is>
-          <t>arthur</t>
+          <t>claibourne</t>
         </is>
       </c>
       <c r="M91" t="inlineStr">
@@ -7741,7 +7736,7 @@
         </is>
       </c>
       <c r="N91" t="n">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="O91" t="inlineStr">
         <is>
@@ -7749,24 +7744,19 @@
         </is>
       </c>
       <c r="P91" t="n">
-        <v>38.92200396</v>
+        <v>38.91305802</v>
       </c>
       <c r="Q91" t="n">
-        <v>-77.03236063</v>
+        <v>-77.02422436000001</v>
       </c>
       <c r="R91" t="inlineStr">
         <is>
-          <t>2500 14TH STREET NW</t>
-        </is>
-      </c>
-      <c r="S91" t="inlineStr">
-        <is>
-          <t>harold mitchell</t>
+          <t>1702 9TH STREET NW</t>
         </is>
       </c>
       <c r="T91" t="inlineStr">
         <is>
-          <t>firearm</t>
+          <t>fire</t>
         </is>
       </c>
     </row>
@@ -7777,7 +7767,7 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>100056434:0:0</t>
+          <t>100053744:0:0</t>
         </is>
       </c>
       <c r="C92" t="n">
@@ -7785,68 +7775,70 @@
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>watson</t>
+          <t>werlich</t>
         </is>
       </c>
       <c r="E92" t="n">
-        <v>100056434</v>
+        <v>100053744</v>
       </c>
       <c r="F92" t="inlineStr">
         <is>
-          <t>100056434:0:0</t>
+          <t>100053744:0:0</t>
         </is>
       </c>
       <c r="G92" t="n">
         <v>2</v>
       </c>
-      <c r="H92" s="3" t="n">
-        <v>28129</v>
-      </c>
       <c r="I92" t="n">
-        <v>2560</v>
+        <v>2572</v>
       </c>
       <c r="J92" t="inlineStr">
         <is>
-          <t>day</t>
+          <t>month</t>
         </is>
       </c>
       <c r="K92" t="inlineStr">
         <is>
-          <t>Claibourne Watson</t>
+          <t>Gladys M. Werlich</t>
         </is>
       </c>
       <c r="L92" t="inlineStr">
         <is>
-          <t>claibourne</t>
+          <t>gladys</t>
         </is>
       </c>
       <c r="M92" t="inlineStr">
         <is>
-          <t>watson</t>
+          <t>werlich</t>
         </is>
       </c>
       <c r="N92" t="n">
-        <v>14</v>
+        <v>85</v>
       </c>
       <c r="O92" t="inlineStr">
         <is>
-          <t>male</t>
+          <t>female</t>
         </is>
       </c>
       <c r="P92" t="n">
-        <v>38.91305802</v>
+        <v>38.9121327</v>
       </c>
       <c r="Q92" t="n">
-        <v>-77.02422436000001</v>
+        <v>-77.0360594</v>
       </c>
       <c r="R92" t="inlineStr">
         <is>
-          <t>1702 9TH STREET NW</t>
+          <t>1625 16TH STREET NW</t>
+        </is>
+      </c>
+      <c r="S92" t="inlineStr">
+        <is>
+          <t>frank mason</t>
         </is>
       </c>
       <c r="T92" t="inlineStr">
         <is>
-          <t>fire</t>
+          <t>unknown</t>
         </is>
       </c>
     </row>
@@ -7857,7 +7849,7 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>100053744:0:0</t>
+          <t>100054118:0:0</t>
         </is>
       </c>
       <c r="C93" t="n">
@@ -7865,70 +7857,68 @@
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>werlich</t>
+          <t>whitehead</t>
         </is>
       </c>
       <c r="E93" t="n">
-        <v>100053744</v>
+        <v>100054118</v>
       </c>
       <c r="F93" t="inlineStr">
         <is>
-          <t>100053744:0:0</t>
+          <t>100054118:0:0</t>
         </is>
       </c>
       <c r="G93" t="n">
         <v>2</v>
       </c>
+      <c r="H93" s="3" t="n">
+        <v>28167</v>
+      </c>
       <c r="I93" t="n">
-        <v>2572</v>
+        <v>2598</v>
       </c>
       <c r="J93" t="inlineStr">
         <is>
-          <t>month</t>
+          <t>day</t>
         </is>
       </c>
       <c r="K93" t="inlineStr">
         <is>
-          <t>Gladys M. Werlich</t>
+          <t>Ralph Whitehead</t>
         </is>
       </c>
       <c r="L93" t="inlineStr">
         <is>
-          <t>gladys</t>
+          <t>ralph</t>
         </is>
       </c>
       <c r="M93" t="inlineStr">
         <is>
-          <t>werlich</t>
+          <t>whitehead</t>
         </is>
       </c>
       <c r="N93" t="n">
-        <v>85</v>
+        <v>32</v>
       </c>
       <c r="O93" t="inlineStr">
         <is>
-          <t>female</t>
+          <t>male</t>
         </is>
       </c>
       <c r="P93" t="n">
-        <v>38.9121327</v>
+        <v>38.85976209</v>
       </c>
       <c r="Q93" t="n">
-        <v>-77.0360594</v>
+        <v>-76.99535457</v>
       </c>
       <c r="R93" t="inlineStr">
         <is>
-          <t>1625 16TH STREET NW</t>
-        </is>
-      </c>
-      <c r="S93" t="inlineStr">
-        <is>
-          <t>frank mason</t>
+          <t>2501 MARTIN LUTHER KING JR AVENUE SE</t>
         </is>
       </c>
       <c r="T93" t="inlineStr">
         <is>
-          <t>unknown</t>
+          <t>firearm</t>
         </is>
       </c>
     </row>
@@ -7939,7 +7929,7 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>100054118:0:0</t>
+          <t>100044168:0:0</t>
         </is>
       </c>
       <c r="C94" t="n">
@@ -7947,25 +7937,25 @@
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>whitehead</t>
+          <t>wilcox</t>
         </is>
       </c>
       <c r="E94" t="n">
-        <v>100054118</v>
+        <v>100044168</v>
       </c>
       <c r="F94" t="inlineStr">
         <is>
-          <t>100054118:0:0</t>
+          <t>100044168:0:0</t>
         </is>
       </c>
       <c r="G94" t="n">
         <v>2</v>
       </c>
       <c r="H94" s="3" t="n">
-        <v>28167</v>
+        <v>28465</v>
       </c>
       <c r="I94" t="n">
-        <v>2598</v>
+        <v>2896</v>
       </c>
       <c r="J94" t="inlineStr">
         <is>
@@ -7974,21 +7964,21 @@
       </c>
       <c r="K94" t="inlineStr">
         <is>
-          <t>Ralph Whitehead</t>
+          <t>Napolen B. Wilcox</t>
         </is>
       </c>
       <c r="L94" t="inlineStr">
         <is>
-          <t>ralph</t>
+          <t>napolen</t>
         </is>
       </c>
       <c r="M94" t="inlineStr">
         <is>
-          <t>whitehead</t>
+          <t>wilcox</t>
         </is>
       </c>
       <c r="N94" t="n">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="O94" t="inlineStr">
         <is>
@@ -7996,19 +7986,24 @@
         </is>
       </c>
       <c r="P94" t="n">
-        <v>38.85976209</v>
+        <v>38.8840648592851</v>
       </c>
       <c r="Q94" t="n">
-        <v>-76.99535457</v>
+        <v>-76.95686087735351</v>
       </c>
       <c r="R94" t="inlineStr">
         <is>
-          <t>2501 MARTIN LUTHER KING JR AVENUE SE</t>
+          <t>3417 MINNESOTA AVENUE SE</t>
+        </is>
+      </c>
+      <c r="S94" t="inlineStr">
+        <is>
+          <t>charles alexander philips</t>
         </is>
       </c>
       <c r="T94" t="inlineStr">
         <is>
-          <t>firearm</t>
+          <t>knife</t>
         </is>
       </c>
     </row>
@@ -8019,33 +8014,33 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>100044168:0:0</t>
+          <t>100040692:0:0</t>
         </is>
       </c>
       <c r="C95" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>wilcox</t>
+          <t>williams</t>
         </is>
       </c>
       <c r="E95" t="n">
-        <v>100044168</v>
+        <v>100040692</v>
       </c>
       <c r="F95" t="inlineStr">
         <is>
-          <t>100044168:0:0</t>
+          <t>100040692:0:0</t>
         </is>
       </c>
       <c r="G95" t="n">
         <v>2</v>
       </c>
       <c r="H95" s="3" t="n">
-        <v>28465</v>
+        <v>28463</v>
       </c>
       <c r="I95" t="n">
-        <v>2896</v>
+        <v>2894</v>
       </c>
       <c r="J95" t="inlineStr">
         <is>
@@ -8054,46 +8049,35 @@
       </c>
       <c r="K95" t="inlineStr">
         <is>
-          <t>Napolen B. Wilcox</t>
+          <t>Edward Williams</t>
         </is>
       </c>
       <c r="L95" t="inlineStr">
         <is>
-          <t>napolen</t>
+          <t>edward</t>
         </is>
       </c>
       <c r="M95" t="inlineStr">
         <is>
-          <t>wilcox</t>
+          <t>williams</t>
         </is>
       </c>
       <c r="N95" t="n">
-        <v>43</v>
+        <v>25</v>
       </c>
       <c r="O95" t="inlineStr">
         <is>
           <t>male</t>
         </is>
       </c>
-      <c r="P95" t="n">
-        <v>38.8840648592851</v>
-      </c>
-      <c r="Q95" t="n">
-        <v>-76.95686087735351</v>
-      </c>
       <c r="R95" t="inlineStr">
         <is>
-          <t>3417 MINNESOTA AVENUE SE</t>
-        </is>
-      </c>
-      <c r="S95" t="inlineStr">
-        <is>
-          <t>charles alexander philips</t>
+          <t>Fort Dupont Park SE</t>
         </is>
       </c>
       <c r="T95" t="inlineStr">
         <is>
-          <t>knife</t>
+          <t>firearm</t>
         </is>
       </c>
     </row>
@@ -8180,11 +8164,11 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>100040692:0:0</t>
+          <t>100063749:1:0</t>
         </is>
       </c>
       <c r="C97" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D97" t="inlineStr">
         <is>
@@ -8192,21 +8176,21 @@
         </is>
       </c>
       <c r="E97" t="n">
-        <v>100040692</v>
+        <v>100063749</v>
       </c>
       <c r="F97" t="inlineStr">
         <is>
-          <t>100040692:0:0</t>
+          <t>100063749:1:0</t>
         </is>
       </c>
       <c r="G97" t="n">
         <v>2</v>
       </c>
       <c r="H97" s="3" t="n">
-        <v>28463</v>
+        <v>28221</v>
       </c>
       <c r="I97" t="n">
-        <v>2894</v>
+        <v>2652</v>
       </c>
       <c r="J97" t="inlineStr">
         <is>
@@ -8215,12 +8199,12 @@
       </c>
       <c r="K97" t="inlineStr">
         <is>
-          <t>Edward Williams</t>
+          <t>Haywood Williams</t>
         </is>
       </c>
       <c r="L97" t="inlineStr">
         <is>
-          <t>edward</t>
+          <t>haywood</t>
         </is>
       </c>
       <c r="M97" t="inlineStr">
@@ -8229,21 +8213,22 @@
         </is>
       </c>
       <c r="N97" t="n">
-        <v>25</v>
-      </c>
-      <c r="O97" t="inlineStr">
-        <is>
-          <t>male</t>
-        </is>
+        <v>51</v>
+      </c>
+      <c r="P97" t="n">
+        <v>38.90837555</v>
+      </c>
+      <c r="Q97" t="n">
+        <v>-77.01143397</v>
       </c>
       <c r="R97" t="inlineStr">
         <is>
-          <t>Fort Dupont Park SE</t>
+          <t>74 O STREET NW</t>
         </is>
       </c>
       <c r="T97" t="inlineStr">
         <is>
-          <t>firearm</t>
+          <t>blunt object</t>
         </is>
       </c>
     </row>
@@ -8254,7 +8239,7 @@
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>100063749:1:0</t>
+          <t>100057635:0:0</t>
         </is>
       </c>
       <c r="C98" t="n">
@@ -8266,21 +8251,21 @@
         </is>
       </c>
       <c r="E98" t="n">
-        <v>100063749</v>
+        <v>100057635</v>
       </c>
       <c r="F98" t="inlineStr">
         <is>
-          <t>100063749:1:0</t>
+          <t>100057635:0:0</t>
         </is>
       </c>
       <c r="G98" t="n">
         <v>2</v>
       </c>
       <c r="H98" s="3" t="n">
-        <v>28221</v>
+        <v>28188</v>
       </c>
       <c r="I98" t="n">
-        <v>2652</v>
+        <v>2619</v>
       </c>
       <c r="J98" t="inlineStr">
         <is>
@@ -8289,12 +8274,12 @@
       </c>
       <c r="K98" t="inlineStr">
         <is>
-          <t>Haywood Williams</t>
+          <t>Jospeh Gregory Williams</t>
         </is>
       </c>
       <c r="L98" t="inlineStr">
         <is>
-          <t>haywood</t>
+          <t>jospeh</t>
         </is>
       </c>
       <c r="M98" t="inlineStr">
@@ -8303,22 +8288,27 @@
         </is>
       </c>
       <c r="N98" t="n">
-        <v>51</v>
+        <v>27</v>
+      </c>
+      <c r="O98" t="inlineStr">
+        <is>
+          <t>male</t>
+        </is>
       </c>
       <c r="P98" t="n">
-        <v>38.90837555</v>
+        <v>38.9542359408298</v>
       </c>
       <c r="Q98" t="n">
-        <v>-77.01143397</v>
+        <v>-77.0222109642604</v>
       </c>
       <c r="R98" t="inlineStr">
         <is>
-          <t>74 O STREET NW</t>
+          <t>7TH STREET NW AND INGRAHAM STREET NW</t>
         </is>
       </c>
       <c r="T98" t="inlineStr">
         <is>
-          <t>blunt object</t>
+          <t>handgun</t>
         </is>
       </c>
     </row>
@@ -8329,33 +8319,33 @@
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>100057635:0:0</t>
+          <t>100009032:1:0</t>
         </is>
       </c>
       <c r="C99" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>williams</t>
+          <t>wilson</t>
         </is>
       </c>
       <c r="E99" t="n">
-        <v>100057635</v>
+        <v>100067595</v>
       </c>
       <c r="F99" t="inlineStr">
         <is>
-          <t>100057635:0:0</t>
+          <t>100067595:0:0</t>
         </is>
       </c>
       <c r="G99" t="n">
         <v>2</v>
       </c>
       <c r="H99" s="3" t="n">
-        <v>28188</v>
+        <v>28240</v>
       </c>
       <c r="I99" t="n">
-        <v>2619</v>
+        <v>2671</v>
       </c>
       <c r="J99" t="inlineStr">
         <is>
@@ -8364,17 +8354,17 @@
       </c>
       <c r="K99" t="inlineStr">
         <is>
-          <t>Jospeh Gregory Williams</t>
+          <t>Bruce W. Wilson</t>
         </is>
       </c>
       <c r="L99" t="inlineStr">
         <is>
-          <t>jospeh</t>
+          <t>bruce</t>
         </is>
       </c>
       <c r="M99" t="inlineStr">
         <is>
-          <t>williams</t>
+          <t>wilson</t>
         </is>
       </c>
       <c r="N99" t="n">
@@ -8386,19 +8376,24 @@
         </is>
       </c>
       <c r="P99" t="n">
-        <v>38.9542359408298</v>
+        <v>38.84024184</v>
       </c>
       <c r="Q99" t="n">
-        <v>-77.0222109642604</v>
+        <v>-76.98708322</v>
       </c>
       <c r="R99" t="inlineStr">
         <is>
-          <t>7TH STREET NW AND INGRAHAM STREET NW</t>
+          <t>1324 MISSISSIPPI AVENUE SE</t>
+        </is>
+      </c>
+      <c r="S99" t="inlineStr">
+        <is>
+          <t>avon alexander</t>
         </is>
       </c>
       <c r="T99" t="inlineStr">
         <is>
-          <t>handgun</t>
+          <t>unknown</t>
         </is>
       </c>
     </row>
@@ -8421,22 +8416,22 @@
         </is>
       </c>
       <c r="E100" t="n">
-        <v>100026075</v>
+        <v>100009032</v>
       </c>
       <c r="F100" t="inlineStr">
         <is>
-          <t>100026075:0:0</t>
+          <t>100009032:1:0</t>
         </is>
       </c>
       <c r="G100" t="n">
         <v>2</v>
       </c>
       <c r="I100" t="n">
-        <v>2661</v>
+        <v>2739</v>
       </c>
       <c r="J100" t="inlineStr">
         <is>
-          <t>month</t>
+          <t>year</t>
         </is>
       </c>
       <c r="K100" t="inlineStr">
@@ -8459,25 +8454,9 @@
           <t>male</t>
         </is>
       </c>
-      <c r="P100" t="n">
-        <v>38.91674538</v>
-      </c>
-      <c r="Q100" t="n">
-        <v>-77.09085428</v>
-      </c>
-      <c r="R100" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="S100" t="inlineStr">
-        <is>
-          <t>avon c  alexander</t>
-        </is>
-      </c>
       <c r="T100" t="inlineStr">
         <is>
-          <t>handgun</t>
+          <t>firearm</t>
         </is>
       </c>
     </row>
@@ -8500,25 +8479,22 @@
         </is>
       </c>
       <c r="E101" t="n">
-        <v>100067595</v>
+        <v>100026075</v>
       </c>
       <c r="F101" t="inlineStr">
         <is>
-          <t>100067595:0:0</t>
+          <t>100026075:0:0</t>
         </is>
       </c>
       <c r="G101" t="n">
         <v>2</v>
       </c>
-      <c r="H101" s="3" t="n">
-        <v>28240</v>
-      </c>
       <c r="I101" t="n">
-        <v>2671</v>
+        <v>2661</v>
       </c>
       <c r="J101" t="inlineStr">
         <is>
-          <t>day</t>
+          <t>month</t>
         </is>
       </c>
       <c r="K101" t="inlineStr">
@@ -8536,33 +8512,30 @@
           <t>wilson</t>
         </is>
       </c>
-      <c r="N101" t="n">
-        <v>27</v>
-      </c>
       <c r="O101" t="inlineStr">
         <is>
           <t>male</t>
         </is>
       </c>
       <c r="P101" t="n">
-        <v>38.84024184</v>
+        <v>38.91674538</v>
       </c>
       <c r="Q101" t="n">
-        <v>-76.98708322</v>
+        <v>-77.09085428</v>
       </c>
       <c r="R101" t="inlineStr">
         <is>
-          <t>1324 MISSISSIPPI AVENUE SE</t>
+          <t>None</t>
         </is>
       </c>
       <c r="S101" t="inlineStr">
         <is>
-          <t>avon alexander</t>
+          <t>avon c  alexander</t>
         </is>
       </c>
       <c r="T101" t="inlineStr">
         <is>
-          <t>unknown</t>
+          <t>handgun</t>
         </is>
       </c>
     </row>
@@ -8585,11 +8558,11 @@
         </is>
       </c>
       <c r="E102" t="n">
-        <v>100018007</v>
+        <v>100066856</v>
       </c>
       <c r="F102" t="inlineStr">
         <is>
-          <t>100018007:0:0</t>
+          <t>100066856:0:0</t>
         </is>
       </c>
       <c r="G102" t="n">
@@ -8622,7 +8595,7 @@
         </is>
       </c>
       <c r="N102" t="n">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="O102" t="inlineStr">
         <is>
@@ -8630,14 +8603,14 @@
         </is>
       </c>
       <c r="P102" t="n">
-        <v>38.82624632</v>
+        <v>38.82584422</v>
       </c>
       <c r="Q102" t="n">
-        <v>-77.01328795000001</v>
+        <v>-77.01287191</v>
       </c>
       <c r="R102" t="inlineStr">
         <is>
-          <t>205 ELMIRA STREET SW</t>
+          <t>200 ELMIRA STREET SW</t>
         </is>
       </c>
       <c r="S102" t="inlineStr">
@@ -8670,22 +8643,22 @@
         </is>
       </c>
       <c r="E103" t="n">
-        <v>100009032</v>
+        <v>100009259</v>
       </c>
       <c r="F103" t="inlineStr">
         <is>
-          <t>100009032:1:0</t>
+          <t>100009259:1:0</t>
         </is>
       </c>
       <c r="G103" t="n">
         <v>2</v>
       </c>
       <c r="I103" t="n">
-        <v>2739</v>
+        <v>2722</v>
       </c>
       <c r="J103" t="inlineStr">
         <is>
-          <t>year</t>
+          <t>month</t>
         </is>
       </c>
       <c r="K103" t="inlineStr">
@@ -8733,11 +8706,11 @@
         </is>
       </c>
       <c r="E104" t="n">
-        <v>100066856</v>
+        <v>100018007</v>
       </c>
       <c r="F104" t="inlineStr">
         <is>
-          <t>100066856:0:0</t>
+          <t>100018007:0:0</t>
         </is>
       </c>
       <c r="G104" t="n">
@@ -8770,7 +8743,7 @@
         </is>
       </c>
       <c r="N104" t="n">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="O104" t="inlineStr">
         <is>
@@ -8778,14 +8751,14 @@
         </is>
       </c>
       <c r="P104" t="n">
-        <v>38.82584422</v>
+        <v>38.82624632</v>
       </c>
       <c r="Q104" t="n">
-        <v>-77.01287191</v>
+        <v>-77.01328795000001</v>
       </c>
       <c r="R104" t="inlineStr">
         <is>
-          <t>200 ELMIRA STREET SW</t>
+          <t>205 ELMIRA STREET SW</t>
         </is>
       </c>
       <c r="S104" t="inlineStr">
@@ -8818,27 +8791,30 @@
         </is>
       </c>
       <c r="E105" t="n">
-        <v>100009259</v>
+        <v>100018689</v>
       </c>
       <c r="F105" t="inlineStr">
         <is>
-          <t>100009259:1:0</t>
+          <t>100018689:0:0</t>
         </is>
       </c>
       <c r="G105" t="n">
         <v>2</v>
       </c>
+      <c r="H105" s="3" t="n">
+        <v>28240</v>
+      </c>
       <c r="I105" t="n">
-        <v>2722</v>
+        <v>2671</v>
       </c>
       <c r="J105" t="inlineStr">
         <is>
-          <t>month</t>
+          <t>day</t>
         </is>
       </c>
       <c r="K105" t="inlineStr">
         <is>
-          <t>Bruce W. Wilson</t>
+          <t>Bruce Wilson</t>
         </is>
       </c>
       <c r="L105" t="inlineStr">
@@ -8854,6 +8830,22 @@
       <c r="O105" t="inlineStr">
         <is>
           <t>male</t>
+        </is>
+      </c>
+      <c r="P105" t="n">
+        <v>38.8260509424163</v>
+      </c>
+      <c r="Q105" t="n">
+        <v>-77.0132524953315</v>
+      </c>
+      <c r="R105" t="inlineStr">
+        <is>
+          <t>ELMIRA STREET SW FROM MARTIN LUTHER KING JR AVENUE SW TO MARTIN LUTHER KING JR AVENUE SW</t>
+        </is>
+      </c>
+      <c r="S105" t="inlineStr">
+        <is>
+          <t>avon c  alexander</t>
         </is>
       </c>
       <c r="T105" t="inlineStr">
@@ -8869,33 +8861,33 @@
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>100009032:1:0</t>
+          <t>100019803:0:0</t>
         </is>
       </c>
       <c r="C106" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D106" t="inlineStr">
         <is>
-          <t>wilson</t>
+          <t>woodward</t>
         </is>
       </c>
       <c r="E106" t="n">
-        <v>100018689</v>
+        <v>100019803</v>
       </c>
       <c r="F106" t="inlineStr">
         <is>
-          <t>100018689:0:0</t>
+          <t>100019803:0:0</t>
         </is>
       </c>
       <c r="G106" t="n">
         <v>2</v>
       </c>
       <c r="H106" s="3" t="n">
-        <v>28240</v>
+        <v>28355</v>
       </c>
       <c r="I106" t="n">
-        <v>2671</v>
+        <v>2786</v>
       </c>
       <c r="J106" t="inlineStr">
         <is>
@@ -8904,18 +8896,21 @@
       </c>
       <c r="K106" t="inlineStr">
         <is>
-          <t>Bruce Wilson</t>
+          <t>Charles Hamilton Woodward</t>
         </is>
       </c>
       <c r="L106" t="inlineStr">
         <is>
-          <t>bruce</t>
+          <t>charles</t>
         </is>
       </c>
       <c r="M106" t="inlineStr">
         <is>
-          <t>wilson</t>
-        </is>
+          <t>woodward</t>
+        </is>
+      </c>
+      <c r="N106" t="n">
+        <v>24</v>
       </c>
       <c r="O106" t="inlineStr">
         <is>
@@ -8923,19 +8918,14 @@
         </is>
       </c>
       <c r="P106" t="n">
-        <v>38.8260509424163</v>
+        <v>38.8606803729819</v>
       </c>
       <c r="Q106" t="n">
-        <v>-77.0132524953315</v>
+        <v>-76.9693260907099</v>
       </c>
       <c r="R106" t="inlineStr">
         <is>
-          <t>ELMIRA STREET SW FROM MARTIN LUTHER KING JR AVENUE SW TO MARTIN LUTHER KING JR AVENUE SW</t>
-        </is>
-      </c>
-      <c r="S106" t="inlineStr">
-        <is>
-          <t>avon c  alexander</t>
+          <t>2501 GOOD HOPE ROAD SE</t>
         </is>
       </c>
       <c r="T106" t="inlineStr">
@@ -8951,7 +8941,7 @@
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>100019803:0:0</t>
+          <t>100016342:0:0</t>
         </is>
       </c>
       <c r="C107" t="n">
@@ -8959,25 +8949,25 @@
       </c>
       <c r="D107" t="inlineStr">
         <is>
-          <t>woodward</t>
+          <t>worthy</t>
         </is>
       </c>
       <c r="E107" t="n">
-        <v>100019803</v>
+        <v>100016342</v>
       </c>
       <c r="F107" t="inlineStr">
         <is>
-          <t>100019803:0:0</t>
+          <t>100016342:0:0</t>
         </is>
       </c>
       <c r="G107" t="n">
         <v>2</v>
       </c>
       <c r="H107" s="3" t="n">
-        <v>28355</v>
+        <v>28336</v>
       </c>
       <c r="I107" t="n">
-        <v>2786</v>
+        <v>2767</v>
       </c>
       <c r="J107" t="inlineStr">
         <is>
@@ -8986,21 +8976,21 @@
       </c>
       <c r="K107" t="inlineStr">
         <is>
-          <t>Charles Hamilton Woodward</t>
+          <t>John Worthy</t>
         </is>
       </c>
       <c r="L107" t="inlineStr">
         <is>
-          <t>charles</t>
+          <t>john</t>
         </is>
       </c>
       <c r="M107" t="inlineStr">
         <is>
-          <t>woodward</t>
+          <t>worthy</t>
         </is>
       </c>
       <c r="N107" t="n">
-        <v>24</v>
+        <v>67</v>
       </c>
       <c r="O107" t="inlineStr">
         <is>
@@ -9008,14 +8998,19 @@
         </is>
       </c>
       <c r="P107" t="n">
-        <v>38.8606803729819</v>
+        <v>38.9056454536728</v>
       </c>
       <c r="Q107" t="n">
-        <v>-76.9693260907099</v>
+        <v>-77.02399247492311</v>
       </c>
       <c r="R107" t="inlineStr">
         <is>
-          <t>2501 GOOD HOPE ROAD SE</t>
+          <t>9TH STREET NW AND M STREET NW</t>
+        </is>
+      </c>
+      <c r="S107" t="inlineStr">
+        <is>
+          <t>mary gillespie</t>
         </is>
       </c>
       <c r="T107" t="inlineStr">
@@ -9031,7 +9026,7 @@
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>100016342:0:0</t>
+          <t>100052572:0:0</t>
         </is>
       </c>
       <c r="C108" t="n">
@@ -9039,25 +9034,25 @@
       </c>
       <c r="D108" t="inlineStr">
         <is>
-          <t>worthy</t>
+          <t>wright</t>
         </is>
       </c>
       <c r="E108" t="n">
-        <v>100016342</v>
+        <v>100052572</v>
       </c>
       <c r="F108" t="inlineStr">
         <is>
-          <t>100016342:0:0</t>
+          <t>100052572:0:0</t>
         </is>
       </c>
       <c r="G108" t="n">
         <v>2</v>
       </c>
       <c r="H108" s="3" t="n">
-        <v>28336</v>
+        <v>28159</v>
       </c>
       <c r="I108" t="n">
-        <v>2767</v>
+        <v>2590</v>
       </c>
       <c r="J108" t="inlineStr">
         <is>
@@ -9066,131 +9061,46 @@
       </c>
       <c r="K108" t="inlineStr">
         <is>
-          <t>John Worthy</t>
+          <t>Lenora Wright</t>
         </is>
       </c>
       <c r="L108" t="inlineStr">
         <is>
-          <t>john</t>
+          <t>lenora</t>
         </is>
       </c>
       <c r="M108" t="inlineStr">
         <is>
-          <t>worthy</t>
+          <t>wright</t>
         </is>
       </c>
       <c r="N108" t="n">
-        <v>67</v>
+        <v>21</v>
       </c>
       <c r="O108" t="inlineStr">
         <is>
-          <t>male</t>
+          <t>female</t>
         </is>
       </c>
       <c r="P108" t="n">
-        <v>38.9056454536728</v>
+        <v>38.8796229150195</v>
       </c>
       <c r="Q108" t="n">
-        <v>-77.02399247492311</v>
+        <v>-76.9320514841373</v>
       </c>
       <c r="R108" t="inlineStr">
         <is>
-          <t>9TH STREET NW AND M STREET NW</t>
-        </is>
-      </c>
-      <c r="S108" t="inlineStr">
-        <is>
-          <t>mary gillespie</t>
+          <t>HANNA PLACE SE AND BENNING ROAD SE</t>
         </is>
       </c>
       <c r="T108" t="inlineStr">
         <is>
-          <t>firearm</t>
-        </is>
-      </c>
-    </row>
-    <row r="109">
-      <c r="A109">
-        <f>MOD(IF($B109 = $B108, $A108, $A108 + 1), 2)</f>
-        <v/>
-      </c>
-      <c r="B109" t="inlineStr">
-        <is>
-          <t>100052572:0:0</t>
-        </is>
-      </c>
-      <c r="C109" t="n">
-        <v>1</v>
-      </c>
-      <c r="D109" t="inlineStr">
-        <is>
-          <t>wright</t>
-        </is>
-      </c>
-      <c r="E109" t="n">
-        <v>100052572</v>
-      </c>
-      <c r="F109" t="inlineStr">
-        <is>
-          <t>100052572:0:0</t>
-        </is>
-      </c>
-      <c r="G109" t="n">
-        <v>2</v>
-      </c>
-      <c r="H109" s="3" t="n">
-        <v>28159</v>
-      </c>
-      <c r="I109" t="n">
-        <v>2590</v>
-      </c>
-      <c r="J109" t="inlineStr">
-        <is>
-          <t>day</t>
-        </is>
-      </c>
-      <c r="K109" t="inlineStr">
-        <is>
-          <t>Lenora Wright</t>
-        </is>
-      </c>
-      <c r="L109" t="inlineStr">
-        <is>
-          <t>lenora</t>
-        </is>
-      </c>
-      <c r="M109" t="inlineStr">
-        <is>
-          <t>wright</t>
-        </is>
-      </c>
-      <c r="N109" t="n">
-        <v>21</v>
-      </c>
-      <c r="O109" t="inlineStr">
-        <is>
-          <t>female</t>
-        </is>
-      </c>
-      <c r="P109" t="n">
-        <v>38.8796229150195</v>
-      </c>
-      <c r="Q109" t="n">
-        <v>-76.9320514841373</v>
-      </c>
-      <c r="R109" t="inlineStr">
-        <is>
-          <t>HANNA PLACE SE AND BENNING ROAD SE</t>
-        </is>
-      </c>
-      <c r="T109" t="inlineStr">
-        <is>
           <t>strangulation</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A2:T109">
+  <conditionalFormatting sqref="A2:T108">
     <cfRule type="expression" priority="1" dxfId="0">
       <formula>$A2 = 0</formula>
     </cfRule>

</xml_diff>

<commit_message>
review special cases and fixes to sql for offender demographics
</commit_message>
<xml_diff>
--- a/top_clusters.xlsx
+++ b/top_clusters.xlsx
@@ -447,7 +447,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T108"/>
+  <dimension ref="A1:T111"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1015,11 +1015,11 @@
         </is>
       </c>
       <c r="E8" t="n">
-        <v>100033633</v>
+        <v>100033844</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>100033633:0:0</t>
+          <t>100033844:0:0</t>
         </is>
       </c>
       <c r="G8" t="n">
@@ -1051,9 +1051,6 @@
           <t>braxton</t>
         </is>
       </c>
-      <c r="N8" t="n">
-        <v>84</v>
-      </c>
       <c r="O8" t="inlineStr">
         <is>
           <t>female</t>
@@ -1061,7 +1058,7 @@
       </c>
       <c r="R8" t="inlineStr">
         <is>
-          <t>Edith M. Haydon Pavilion, St. Elizabeths Hospital</t>
+          <t>St. Elizabeths Hospital</t>
         </is>
       </c>
       <c r="S8" t="inlineStr">
@@ -1071,7 +1068,7 @@
       </c>
       <c r="T8" t="inlineStr">
         <is>
-          <t>personal weapon</t>
+          <t>blunt object</t>
         </is>
       </c>
     </row>
@@ -1094,11 +1091,11 @@
         </is>
       </c>
       <c r="E9" t="n">
-        <v>100033844</v>
+        <v>100033633</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>100033844:0:0</t>
+          <t>100033633:0:0</t>
         </is>
       </c>
       <c r="G9" t="n">
@@ -1130,6 +1127,9 @@
           <t>braxton</t>
         </is>
       </c>
+      <c r="N9" t="n">
+        <v>84</v>
+      </c>
       <c r="O9" t="inlineStr">
         <is>
           <t>female</t>
@@ -1137,7 +1137,7 @@
       </c>
       <c r="R9" t="inlineStr">
         <is>
-          <t>St. Elizabeths Hospital</t>
+          <t>Edith M. Haydon Pavilion, St. Elizabeths Hospital</t>
         </is>
       </c>
       <c r="S9" t="inlineStr">
@@ -1147,7 +1147,7 @@
       </c>
       <c r="T9" t="inlineStr">
         <is>
-          <t>blunt object</t>
+          <t>personal weapon</t>
         </is>
       </c>
     </row>
@@ -2028,11 +2028,11 @@
         </is>
       </c>
       <c r="E21" t="n">
-        <v>100068117</v>
+        <v>100000119</v>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>100068117:0:0</t>
+          <t>100000119:0:0</t>
         </is>
       </c>
       <c r="G21" t="n">
@@ -2073,14 +2073,14 @@
         </is>
       </c>
       <c r="P21" t="n">
-        <v>38.887589465233</v>
+        <v>38.88682291</v>
       </c>
       <c r="Q21" t="n">
-        <v>-76.98076325387819</v>
+        <v>-76.97917206</v>
       </c>
       <c r="R21" t="inlineStr">
         <is>
-          <t>17TH STREET SE AND INDEPENDENCE AVENUE SE</t>
+          <t>1740 BAY STREET SE</t>
         </is>
       </c>
       <c r="S21" t="inlineStr">
@@ -2113,11 +2113,11 @@
         </is>
       </c>
       <c r="E22" t="n">
-        <v>100000119</v>
+        <v>100068117</v>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>100000119:0:0</t>
+          <t>100068117:0:0</t>
         </is>
       </c>
       <c r="G22" t="n">
@@ -2158,14 +2158,14 @@
         </is>
       </c>
       <c r="P22" t="n">
-        <v>38.88682291</v>
+        <v>38.887589465233</v>
       </c>
       <c r="Q22" t="n">
-        <v>-76.97917206</v>
+        <v>-76.98076325387819</v>
       </c>
       <c r="R22" t="inlineStr">
         <is>
-          <t>1740 BAY STREET SE</t>
+          <t>17TH STREET SE AND INDEPENDENCE AVENUE SE</t>
         </is>
       </c>
       <c r="S22" t="inlineStr">
@@ -2442,11 +2442,11 @@
         </is>
       </c>
       <c r="E26" t="n">
-        <v>100016342</v>
+        <v>100010846</v>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>100016342:1:0</t>
+          <t>100010846:0:0</t>
         </is>
       </c>
       <c r="G26" t="n">
@@ -2479,21 +2479,27 @@
         </is>
       </c>
       <c r="N26" t="n">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="O26" t="inlineStr">
         <is>
           <t>male</t>
         </is>
       </c>
-      <c r="S26" t="inlineStr">
-        <is>
-          <t>leon david morton</t>
+      <c r="P26" t="n">
+        <v>38.9056454536728</v>
+      </c>
+      <c r="Q26" t="n">
+        <v>-77.02399247492311</v>
+      </c>
+      <c r="R26" t="inlineStr">
+        <is>
+          <t>9TH STREET NW AND M STREET NW</t>
         </is>
       </c>
       <c r="T26" t="inlineStr">
         <is>
-          <t>firearm</t>
+          <t>unknown</t>
         </is>
       </c>
     </row>
@@ -2516,11 +2522,11 @@
         </is>
       </c>
       <c r="E27" t="n">
-        <v>100010846</v>
+        <v>100015333</v>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>100010846:0:0</t>
+          <t>100015333:1:0</t>
         </is>
       </c>
       <c r="G27" t="n">
@@ -2553,7 +2559,7 @@
         </is>
       </c>
       <c r="N27" t="n">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O27" t="inlineStr">
         <is>
@@ -2561,14 +2567,19 @@
         </is>
       </c>
       <c r="P27" t="n">
-        <v>38.9056454536728</v>
+        <v>38.9072362908274</v>
       </c>
       <c r="Q27" t="n">
-        <v>-77.02399247492311</v>
+        <v>-77.0229447208942</v>
       </c>
       <c r="R27" t="inlineStr">
         <is>
-          <t>9TH STREET NW AND M STREET NW</t>
+          <t>8TH STREET NW AND N STREET NW</t>
+        </is>
+      </c>
+      <c r="S27" t="inlineStr">
+        <is>
+          <t>leon david morton</t>
         </is>
       </c>
       <c r="T27" t="inlineStr">
@@ -2596,11 +2607,11 @@
         </is>
       </c>
       <c r="E28" t="n">
-        <v>100015333</v>
+        <v>100016342</v>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>100015333:1:0</t>
+          <t>100016342:1:0</t>
         </is>
       </c>
       <c r="G28" t="n">
@@ -2640,17 +2651,6 @@
           <t>male</t>
         </is>
       </c>
-      <c r="P28" t="n">
-        <v>38.9072362908274</v>
-      </c>
-      <c r="Q28" t="n">
-        <v>-77.0229447208942</v>
-      </c>
-      <c r="R28" t="inlineStr">
-        <is>
-          <t>8TH STREET NW AND N STREET NW</t>
-        </is>
-      </c>
       <c r="S28" t="inlineStr">
         <is>
           <t>leon david morton</t>
@@ -2658,7 +2658,7 @@
       </c>
       <c r="T28" t="inlineStr">
         <is>
-          <t>unknown</t>
+          <t>firearm</t>
         </is>
       </c>
     </row>
@@ -3152,22 +3152,22 @@
         </is>
       </c>
       <c r="E35" t="n">
-        <v>100041397</v>
+        <v>100018683</v>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>100041397:0:0</t>
+          <t>100018683:0:0</t>
         </is>
       </c>
       <c r="G35" t="n">
         <v>2</v>
       </c>
       <c r="I35" t="n">
-        <v>2739</v>
+        <v>2692</v>
       </c>
       <c r="J35" t="inlineStr">
         <is>
-          <t>year</t>
+          <t>month</t>
         </is>
       </c>
       <c r="K35" t="inlineStr">
@@ -3215,22 +3215,25 @@
         </is>
       </c>
       <c r="E36" t="n">
-        <v>100018683</v>
+        <v>100004364</v>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>100018683:0:0</t>
+          <t>100004364:0:0</t>
         </is>
       </c>
       <c r="G36" t="n">
         <v>2</v>
       </c>
+      <c r="H36" s="3" t="n">
+        <v>28257</v>
+      </c>
       <c r="I36" t="n">
-        <v>2692</v>
+        <v>2688</v>
       </c>
       <c r="J36" t="inlineStr">
         <is>
-          <t>month</t>
+          <t>day</t>
         </is>
       </c>
       <c r="K36" t="inlineStr">
@@ -3248,14 +3251,28 @@
           <t>goodarzi</t>
         </is>
       </c>
+      <c r="N36" t="n">
+        <v>36</v>
+      </c>
+      <c r="O36" t="inlineStr">
+        <is>
+          <t>male</t>
+        </is>
+      </c>
+      <c r="P36" t="n">
+        <v>38.90917468</v>
+      </c>
+      <c r="Q36" t="n">
+        <v>-77.08658868000001</v>
+      </c>
       <c r="R36" t="inlineStr">
         <is>
-          <t>Rotunda Restaurant, Capitol Hill</t>
+          <t>4545 MACARTHUR BOULEVARD NW</t>
         </is>
       </c>
       <c r="T36" t="inlineStr">
         <is>
-          <t>unknown</t>
+          <t>handgun</t>
         </is>
       </c>
     </row>
@@ -3278,25 +3295,22 @@
         </is>
       </c>
       <c r="E37" t="n">
-        <v>100002194</v>
+        <v>100041397</v>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>100002194:0:0</t>
+          <t>100041397:0:0</t>
         </is>
       </c>
       <c r="G37" t="n">
         <v>2</v>
       </c>
-      <c r="H37" s="3" t="n">
-        <v>28261</v>
-      </c>
       <c r="I37" t="n">
-        <v>2692</v>
+        <v>2739</v>
       </c>
       <c r="J37" t="inlineStr">
         <is>
-          <t>day</t>
+          <t>year</t>
         </is>
       </c>
       <c r="K37" t="inlineStr">
@@ -3314,19 +3328,14 @@
           <t>goodarzi</t>
         </is>
       </c>
-      <c r="O37" t="inlineStr">
-        <is>
-          <t>male</t>
-        </is>
-      </c>
       <c r="R37" t="inlineStr">
         <is>
-          <t>Rotunda restaurant</t>
+          <t>Rotunda Restaurant, Capitol Hill</t>
         </is>
       </c>
       <c r="T37" t="inlineStr">
         <is>
-          <t>firearm</t>
+          <t>unknown</t>
         </is>
       </c>
     </row>
@@ -3349,21 +3358,21 @@
         </is>
       </c>
       <c r="E38" t="n">
-        <v>100004364</v>
+        <v>100002194</v>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>100004364:0:0</t>
+          <t>100002194:0:0</t>
         </is>
       </c>
       <c r="G38" t="n">
         <v>2</v>
       </c>
       <c r="H38" s="3" t="n">
-        <v>28257</v>
+        <v>28261</v>
       </c>
       <c r="I38" t="n">
-        <v>2688</v>
+        <v>2692</v>
       </c>
       <c r="J38" t="inlineStr">
         <is>
@@ -3385,28 +3394,19 @@
           <t>goodarzi</t>
         </is>
       </c>
-      <c r="N38" t="n">
-        <v>36</v>
-      </c>
       <c r="O38" t="inlineStr">
         <is>
           <t>male</t>
         </is>
       </c>
-      <c r="P38" t="n">
-        <v>38.90917468</v>
-      </c>
-      <c r="Q38" t="n">
-        <v>-77.08658868000001</v>
-      </c>
       <c r="R38" t="inlineStr">
         <is>
-          <t>4545 MACARTHUR BOULEVARD NW</t>
+          <t>Rotunda restaurant</t>
         </is>
       </c>
       <c r="T38" t="inlineStr">
         <is>
-          <t>handgun</t>
+          <t>firearm</t>
         </is>
       </c>
     </row>
@@ -5328,21 +5328,21 @@
         </is>
       </c>
       <c r="E62" t="n">
-        <v>100025319</v>
+        <v>100023762</v>
       </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t>100025319:0:0</t>
+          <t>100023762:0:0</t>
         </is>
       </c>
       <c r="G62" t="n">
         <v>2</v>
       </c>
       <c r="H62" s="3" t="n">
-        <v>28381</v>
+        <v>28378</v>
       </c>
       <c r="I62" t="n">
-        <v>2812</v>
+        <v>2809</v>
       </c>
       <c r="J62" t="inlineStr">
         <is>
@@ -5373,19 +5373,19 @@
         </is>
       </c>
       <c r="P62" t="n">
-        <v>38.90163219</v>
+        <v>38.8969193330944</v>
       </c>
       <c r="Q62" t="n">
-        <v>-76.95075158</v>
+        <v>-76.9602617838556</v>
       </c>
       <c r="R62" t="inlineStr">
         <is>
-          <t>709 ANACOSTIA AVENUE NE</t>
+          <t>ANACOSTIA AVENUE NE AND BENNING ROAD NE</t>
         </is>
       </c>
       <c r="T62" t="inlineStr">
         <is>
-          <t>unknown</t>
+          <t>firearm</t>
         </is>
       </c>
     </row>
@@ -5408,21 +5408,21 @@
         </is>
       </c>
       <c r="E63" t="n">
-        <v>100023762</v>
+        <v>100025319</v>
       </c>
       <c r="F63" t="inlineStr">
         <is>
-          <t>100023762:0:0</t>
+          <t>100025319:0:0</t>
         </is>
       </c>
       <c r="G63" t="n">
         <v>2</v>
       </c>
       <c r="H63" s="3" t="n">
-        <v>28378</v>
+        <v>28381</v>
       </c>
       <c r="I63" t="n">
-        <v>2809</v>
+        <v>2812</v>
       </c>
       <c r="J63" t="inlineStr">
         <is>
@@ -5453,19 +5453,19 @@
         </is>
       </c>
       <c r="P63" t="n">
-        <v>38.8969193330944</v>
+        <v>38.90163219</v>
       </c>
       <c r="Q63" t="n">
-        <v>-76.9602617838556</v>
+        <v>-76.95075158</v>
       </c>
       <c r="R63" t="inlineStr">
         <is>
-          <t>ANACOSTIA AVENUE NE AND BENNING ROAD NE</t>
+          <t>709 ANACOSTIA AVENUE NE</t>
         </is>
       </c>
       <c r="T63" t="inlineStr">
         <is>
-          <t>firearm</t>
+          <t>unknown</t>
         </is>
       </c>
     </row>
@@ -6381,11 +6381,11 @@
         </is>
       </c>
       <c r="E75" t="n">
-        <v>100004075</v>
+        <v>100010689</v>
       </c>
       <c r="F75" t="inlineStr">
         <is>
-          <t>100004075:0:0</t>
+          <t>100010689:0:0</t>
         </is>
       </c>
       <c r="G75" t="n">
@@ -6443,7 +6443,7 @@
       </c>
       <c r="T75" t="inlineStr">
         <is>
-          <t>firearm</t>
+          <t>unknown</t>
         </is>
       </c>
     </row>
@@ -6534,11 +6534,11 @@
         </is>
       </c>
       <c r="E77" t="n">
-        <v>100010689</v>
+        <v>100004075</v>
       </c>
       <c r="F77" t="inlineStr">
         <is>
-          <t>100010689:0:0</t>
+          <t>100004075:0:0</t>
         </is>
       </c>
       <c r="G77" t="n">
@@ -6596,7 +6596,7 @@
       </c>
       <c r="T77" t="inlineStr">
         <is>
-          <t>unknown</t>
+          <t>firearm</t>
         </is>
       </c>
     </row>
@@ -8026,25 +8026,22 @@
         </is>
       </c>
       <c r="E95" t="n">
-        <v>100040692</v>
+        <v>100040873</v>
       </c>
       <c r="F95" t="inlineStr">
         <is>
-          <t>100040692:0:0</t>
+          <t>100040873:0:0</t>
         </is>
       </c>
       <c r="G95" t="n">
         <v>2</v>
       </c>
-      <c r="H95" s="3" t="n">
-        <v>28463</v>
-      </c>
       <c r="I95" t="n">
-        <v>2894</v>
+        <v>2906</v>
       </c>
       <c r="J95" t="inlineStr">
         <is>
-          <t>day</t>
+          <t>month</t>
         </is>
       </c>
       <c r="K95" t="inlineStr">
@@ -8072,7 +8069,12 @@
       </c>
       <c r="R95" t="inlineStr">
         <is>
-          <t>Fort Dupont Park SE</t>
+          <t>Fort DuPont Park, SE</t>
+        </is>
+      </c>
+      <c r="S95" t="inlineStr">
+        <is>
+          <t>james m  head</t>
         </is>
       </c>
       <c r="T95" t="inlineStr">
@@ -8100,22 +8102,25 @@
         </is>
       </c>
       <c r="E96" t="n">
-        <v>100040873</v>
+        <v>100040692</v>
       </c>
       <c r="F96" t="inlineStr">
         <is>
-          <t>100040873:0:0</t>
+          <t>100040692:0:0</t>
         </is>
       </c>
       <c r="G96" t="n">
         <v>2</v>
       </c>
+      <c r="H96" s="3" t="n">
+        <v>28463</v>
+      </c>
       <c r="I96" t="n">
-        <v>2906</v>
+        <v>2894</v>
       </c>
       <c r="J96" t="inlineStr">
         <is>
-          <t>month</t>
+          <t>day</t>
         </is>
       </c>
       <c r="K96" t="inlineStr">
@@ -8143,12 +8148,7 @@
       </c>
       <c r="R96" t="inlineStr">
         <is>
-          <t>Fort DuPont Park, SE</t>
-        </is>
-      </c>
-      <c r="S96" t="inlineStr">
-        <is>
-          <t>james m  head</t>
+          <t>Fort Dupont Park SE</t>
         </is>
       </c>
       <c r="T96" t="inlineStr">
@@ -8319,33 +8319,33 @@
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>100009032:1:0</t>
+          <t>100058475:0:0</t>
         </is>
       </c>
       <c r="C99" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>wilson</t>
+          <t>williams</t>
         </is>
       </c>
       <c r="E99" t="n">
-        <v>100067595</v>
+        <v>100058678</v>
       </c>
       <c r="F99" t="inlineStr">
         <is>
-          <t>100067595:0:0</t>
+          <t>100058678:0:0</t>
         </is>
       </c>
       <c r="G99" t="n">
         <v>2</v>
       </c>
       <c r="H99" s="3" t="n">
-        <v>28240</v>
+        <v>28193</v>
       </c>
       <c r="I99" t="n">
-        <v>2671</v>
+        <v>2624</v>
       </c>
       <c r="J99" t="inlineStr">
         <is>
@@ -8354,21 +8354,21 @@
       </c>
       <c r="K99" t="inlineStr">
         <is>
-          <t>Bruce W. Wilson</t>
+          <t>Maurice Williams</t>
         </is>
       </c>
       <c r="L99" t="inlineStr">
         <is>
-          <t>bruce</t>
+          <t>maurice</t>
         </is>
       </c>
       <c r="M99" t="inlineStr">
         <is>
-          <t>wilson</t>
+          <t>williams</t>
         </is>
       </c>
       <c r="N99" t="n">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="O99" t="inlineStr">
         <is>
@@ -8376,24 +8376,19 @@
         </is>
       </c>
       <c r="P99" t="n">
-        <v>38.84024184</v>
+        <v>38.89500269</v>
       </c>
       <c r="Q99" t="n">
-        <v>-76.98708322</v>
+        <v>-77.03135287000001</v>
       </c>
       <c r="R99" t="inlineStr">
         <is>
-          <t>1324 MISSISSIPPI AVENUE SE</t>
-        </is>
-      </c>
-      <c r="S99" t="inlineStr">
-        <is>
-          <t>avon alexander</t>
+          <t>1350 PENNSYLVANIA AVENUE NW</t>
         </is>
       </c>
       <c r="T99" t="inlineStr">
         <is>
-          <t>unknown</t>
+          <t>firearm</t>
         </is>
       </c>
     </row>
@@ -8404,59 +8399,76 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>100009032:1:0</t>
+          <t>100058475:0:0</t>
         </is>
       </c>
       <c r="C100" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>wilson</t>
+          <t>williams</t>
         </is>
       </c>
       <c r="E100" t="n">
-        <v>100009032</v>
+        <v>100058475</v>
       </c>
       <c r="F100" t="inlineStr">
         <is>
-          <t>100009032:1:0</t>
+          <t>100058475:0:0</t>
         </is>
       </c>
       <c r="G100" t="n">
         <v>2</v>
       </c>
+      <c r="H100" s="3" t="n">
+        <v>28193</v>
+      </c>
       <c r="I100" t="n">
-        <v>2739</v>
+        <v>2624</v>
       </c>
       <c r="J100" t="inlineStr">
         <is>
-          <t>year</t>
+          <t>day</t>
         </is>
       </c>
       <c r="K100" t="inlineStr">
         <is>
-          <t>Bruce W. Wilson</t>
+          <t>Maurice Williams</t>
         </is>
       </c>
       <c r="L100" t="inlineStr">
         <is>
-          <t>bruce</t>
+          <t>maurice</t>
         </is>
       </c>
       <c r="M100" t="inlineStr">
         <is>
-          <t>wilson</t>
-        </is>
+          <t>williams</t>
+        </is>
+      </c>
+      <c r="N100" t="n">
+        <v>22</v>
       </c>
       <c r="O100" t="inlineStr">
         <is>
           <t>male</t>
         </is>
       </c>
+      <c r="P100" t="n">
+        <v>38.89500269</v>
+      </c>
+      <c r="Q100" t="n">
+        <v>-77.03135287000001</v>
+      </c>
+      <c r="R100" t="inlineStr">
+        <is>
+          <t>1350 PENNSYLVANIA AVENUE NW</t>
+        </is>
+      </c>
       <c r="T100" t="inlineStr">
         <is>
-          <t>firearm</t>
+          <t>shotgun</t>
         </is>
       </c>
     </row>
@@ -8467,30 +8479,30 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>100009032:1:0</t>
+          <t>100058475:0:0</t>
         </is>
       </c>
       <c r="C101" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>wilson</t>
+          <t>williams</t>
         </is>
       </c>
       <c r="E101" t="n">
-        <v>100026075</v>
+        <v>100059331</v>
       </c>
       <c r="F101" t="inlineStr">
         <is>
-          <t>100026075:0:0</t>
+          <t>100059331:0:0</t>
         </is>
       </c>
       <c r="G101" t="n">
         <v>2</v>
       </c>
       <c r="I101" t="n">
-        <v>2661</v>
+        <v>2631</v>
       </c>
       <c r="J101" t="inlineStr">
         <is>
@@ -8499,18 +8511,21 @@
       </c>
       <c r="K101" t="inlineStr">
         <is>
-          <t>Bruce W. Wilson</t>
+          <t>Maurice Williams</t>
         </is>
       </c>
       <c r="L101" t="inlineStr">
         <is>
-          <t>bruce</t>
+          <t>maurice</t>
         </is>
       </c>
       <c r="M101" t="inlineStr">
         <is>
-          <t>wilson</t>
-        </is>
+          <t>williams</t>
+        </is>
+      </c>
+      <c r="N101" t="n">
+        <v>24</v>
       </c>
       <c r="O101" t="inlineStr">
         <is>
@@ -8518,24 +8533,19 @@
         </is>
       </c>
       <c r="P101" t="n">
-        <v>38.91674538</v>
+        <v>38.89500269</v>
       </c>
       <c r="Q101" t="n">
-        <v>-77.09085428</v>
+        <v>-77.03135287000001</v>
       </c>
       <c r="R101" t="inlineStr">
         <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="S101" t="inlineStr">
-        <is>
-          <t>avon c  alexander</t>
+          <t>1350 PENNSYLVANIA AVENUE NW</t>
         </is>
       </c>
       <c r="T101" t="inlineStr">
         <is>
-          <t>handgun</t>
+          <t>shotgun</t>
         </is>
       </c>
     </row>
@@ -8558,25 +8568,22 @@
         </is>
       </c>
       <c r="E102" t="n">
-        <v>100066856</v>
+        <v>100009032</v>
       </c>
       <c r="F102" t="inlineStr">
         <is>
-          <t>100066856:0:0</t>
+          <t>100009032:1:0</t>
         </is>
       </c>
       <c r="G102" t="n">
         <v>2</v>
       </c>
-      <c r="H102" s="3" t="n">
-        <v>28240</v>
-      </c>
       <c r="I102" t="n">
-        <v>2671</v>
+        <v>2739</v>
       </c>
       <c r="J102" t="inlineStr">
         <is>
-          <t>day</t>
+          <t>year</t>
         </is>
       </c>
       <c r="K102" t="inlineStr">
@@ -8594,33 +8601,14 @@
           <t>wilson</t>
         </is>
       </c>
-      <c r="N102" t="n">
-        <v>27</v>
-      </c>
       <c r="O102" t="inlineStr">
         <is>
           <t>male</t>
         </is>
       </c>
-      <c r="P102" t="n">
-        <v>38.82584422</v>
-      </c>
-      <c r="Q102" t="n">
-        <v>-77.01287191</v>
-      </c>
-      <c r="R102" t="inlineStr">
-        <is>
-          <t>200 ELMIRA STREET SW</t>
-        </is>
-      </c>
-      <c r="S102" t="inlineStr">
-        <is>
-          <t>avon c  alexander</t>
-        </is>
-      </c>
       <c r="T102" t="inlineStr">
         <is>
-          <t>handgun</t>
+          <t>firearm</t>
         </is>
       </c>
     </row>
@@ -8643,22 +8631,25 @@
         </is>
       </c>
       <c r="E103" t="n">
-        <v>100009259</v>
+        <v>100067595</v>
       </c>
       <c r="F103" t="inlineStr">
         <is>
-          <t>100009259:1:0</t>
+          <t>100067595:0:0</t>
         </is>
       </c>
       <c r="G103" t="n">
         <v>2</v>
       </c>
+      <c r="H103" s="3" t="n">
+        <v>28240</v>
+      </c>
       <c r="I103" t="n">
-        <v>2722</v>
+        <v>2671</v>
       </c>
       <c r="J103" t="inlineStr">
         <is>
-          <t>month</t>
+          <t>day</t>
         </is>
       </c>
       <c r="K103" t="inlineStr">
@@ -8676,14 +8667,33 @@
           <t>wilson</t>
         </is>
       </c>
+      <c r="N103" t="n">
+        <v>27</v>
+      </c>
       <c r="O103" t="inlineStr">
         <is>
           <t>male</t>
         </is>
       </c>
+      <c r="P103" t="n">
+        <v>38.84024184</v>
+      </c>
+      <c r="Q103" t="n">
+        <v>-76.98708322</v>
+      </c>
+      <c r="R103" t="inlineStr">
+        <is>
+          <t>1324 MISSISSIPPI AVENUE SE</t>
+        </is>
+      </c>
+      <c r="S103" t="inlineStr">
+        <is>
+          <t>avon alexander</t>
+        </is>
+      </c>
       <c r="T103" t="inlineStr">
         <is>
-          <t>firearm</t>
+          <t>unknown</t>
         </is>
       </c>
     </row>
@@ -8706,25 +8716,22 @@
         </is>
       </c>
       <c r="E104" t="n">
-        <v>100018007</v>
+        <v>100026075</v>
       </c>
       <c r="F104" t="inlineStr">
         <is>
-          <t>100018007:0:0</t>
+          <t>100026075:0:0</t>
         </is>
       </c>
       <c r="G104" t="n">
         <v>2</v>
       </c>
-      <c r="H104" s="3" t="n">
-        <v>28240</v>
-      </c>
       <c r="I104" t="n">
-        <v>2671</v>
+        <v>2661</v>
       </c>
       <c r="J104" t="inlineStr">
         <is>
-          <t>day</t>
+          <t>month</t>
         </is>
       </c>
       <c r="K104" t="inlineStr">
@@ -8742,23 +8749,20 @@
           <t>wilson</t>
         </is>
       </c>
-      <c r="N104" t="n">
-        <v>26</v>
-      </c>
       <c r="O104" t="inlineStr">
         <is>
           <t>male</t>
         </is>
       </c>
       <c r="P104" t="n">
-        <v>38.82624632</v>
+        <v>38.91674538</v>
       </c>
       <c r="Q104" t="n">
-        <v>-77.01328795000001</v>
+        <v>-77.09085428</v>
       </c>
       <c r="R104" t="inlineStr">
         <is>
-          <t>205 ELMIRA STREET SW</t>
+          <t>None</t>
         </is>
       </c>
       <c r="S104" t="inlineStr">
@@ -8791,11 +8795,11 @@
         </is>
       </c>
       <c r="E105" t="n">
-        <v>100018689</v>
+        <v>100018007</v>
       </c>
       <c r="F105" t="inlineStr">
         <is>
-          <t>100018689:0:0</t>
+          <t>100018007:0:0</t>
         </is>
       </c>
       <c r="G105" t="n">
@@ -8814,7 +8818,7 @@
       </c>
       <c r="K105" t="inlineStr">
         <is>
-          <t>Bruce Wilson</t>
+          <t>Bruce W. Wilson</t>
         </is>
       </c>
       <c r="L105" t="inlineStr">
@@ -8827,20 +8831,23 @@
           <t>wilson</t>
         </is>
       </c>
+      <c r="N105" t="n">
+        <v>26</v>
+      </c>
       <c r="O105" t="inlineStr">
         <is>
           <t>male</t>
         </is>
       </c>
       <c r="P105" t="n">
-        <v>38.8260509424163</v>
+        <v>38.82624632</v>
       </c>
       <c r="Q105" t="n">
-        <v>-77.0132524953315</v>
+        <v>-77.01328795000001</v>
       </c>
       <c r="R105" t="inlineStr">
         <is>
-          <t>ELMIRA STREET SW FROM MARTIN LUTHER KING JR AVENUE SW TO MARTIN LUTHER KING JR AVENUE SW</t>
+          <t>205 ELMIRA STREET SW</t>
         </is>
       </c>
       <c r="S105" t="inlineStr">
@@ -8850,7 +8857,7 @@
       </c>
       <c r="T105" t="inlineStr">
         <is>
-          <t>firearm</t>
+          <t>handgun</t>
         </is>
       </c>
     </row>
@@ -8861,33 +8868,33 @@
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>100019803:0:0</t>
+          <t>100009032:1:0</t>
         </is>
       </c>
       <c r="C106" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="D106" t="inlineStr">
         <is>
-          <t>woodward</t>
+          <t>wilson</t>
         </is>
       </c>
       <c r="E106" t="n">
-        <v>100019803</v>
+        <v>100066856</v>
       </c>
       <c r="F106" t="inlineStr">
         <is>
-          <t>100019803:0:0</t>
+          <t>100066856:0:0</t>
         </is>
       </c>
       <c r="G106" t="n">
         <v>2</v>
       </c>
       <c r="H106" s="3" t="n">
-        <v>28355</v>
+        <v>28240</v>
       </c>
       <c r="I106" t="n">
-        <v>2786</v>
+        <v>2671</v>
       </c>
       <c r="J106" t="inlineStr">
         <is>
@@ -8896,21 +8903,21 @@
       </c>
       <c r="K106" t="inlineStr">
         <is>
-          <t>Charles Hamilton Woodward</t>
+          <t>Bruce W. Wilson</t>
         </is>
       </c>
       <c r="L106" t="inlineStr">
         <is>
-          <t>charles</t>
+          <t>bruce</t>
         </is>
       </c>
       <c r="M106" t="inlineStr">
         <is>
-          <t>woodward</t>
+          <t>wilson</t>
         </is>
       </c>
       <c r="N106" t="n">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="O106" t="inlineStr">
         <is>
@@ -8918,19 +8925,24 @@
         </is>
       </c>
       <c r="P106" t="n">
-        <v>38.8606803729819</v>
+        <v>38.82584422</v>
       </c>
       <c r="Q106" t="n">
-        <v>-76.9693260907099</v>
+        <v>-77.01287191</v>
       </c>
       <c r="R106" t="inlineStr">
         <is>
-          <t>2501 GOOD HOPE ROAD SE</t>
+          <t>200 ELMIRA STREET SW</t>
+        </is>
+      </c>
+      <c r="S106" t="inlineStr">
+        <is>
+          <t>avon c  alexander</t>
         </is>
       </c>
       <c r="T106" t="inlineStr">
         <is>
-          <t>firearm</t>
+          <t>handgun</t>
         </is>
       </c>
     </row>
@@ -8941,76 +8953,54 @@
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>100016342:0:0</t>
+          <t>100009032:1:0</t>
         </is>
       </c>
       <c r="C107" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="D107" t="inlineStr">
         <is>
-          <t>worthy</t>
+          <t>wilson</t>
         </is>
       </c>
       <c r="E107" t="n">
-        <v>100016342</v>
+        <v>100009259</v>
       </c>
       <c r="F107" t="inlineStr">
         <is>
-          <t>100016342:0:0</t>
+          <t>100009259:1:0</t>
         </is>
       </c>
       <c r="G107" t="n">
         <v>2</v>
       </c>
-      <c r="H107" s="3" t="n">
-        <v>28336</v>
-      </c>
       <c r="I107" t="n">
-        <v>2767</v>
+        <v>2722</v>
       </c>
       <c r="J107" t="inlineStr">
         <is>
-          <t>day</t>
+          <t>month</t>
         </is>
       </c>
       <c r="K107" t="inlineStr">
         <is>
-          <t>John Worthy</t>
+          <t>Bruce W. Wilson</t>
         </is>
       </c>
       <c r="L107" t="inlineStr">
         <is>
-          <t>john</t>
+          <t>bruce</t>
         </is>
       </c>
       <c r="M107" t="inlineStr">
         <is>
-          <t>worthy</t>
-        </is>
-      </c>
-      <c r="N107" t="n">
-        <v>67</v>
+          <t>wilson</t>
+        </is>
       </c>
       <c r="O107" t="inlineStr">
         <is>
           <t>male</t>
-        </is>
-      </c>
-      <c r="P107" t="n">
-        <v>38.9056454536728</v>
-      </c>
-      <c r="Q107" t="n">
-        <v>-77.02399247492311</v>
-      </c>
-      <c r="R107" t="inlineStr">
-        <is>
-          <t>9TH STREET NW AND M STREET NW</t>
-        </is>
-      </c>
-      <c r="S107" t="inlineStr">
-        <is>
-          <t>mary gillespie</t>
         </is>
       </c>
       <c r="T107" t="inlineStr">
@@ -9026,81 +9016,328 @@
       </c>
       <c r="B108" t="inlineStr">
         <is>
+          <t>100009032:1:0</t>
+        </is>
+      </c>
+      <c r="C108" t="n">
+        <v>7</v>
+      </c>
+      <c r="D108" t="inlineStr">
+        <is>
+          <t>wilson</t>
+        </is>
+      </c>
+      <c r="E108" t="n">
+        <v>100018689</v>
+      </c>
+      <c r="F108" t="inlineStr">
+        <is>
+          <t>100018689:0:0</t>
+        </is>
+      </c>
+      <c r="G108" t="n">
+        <v>2</v>
+      </c>
+      <c r="H108" s="3" t="n">
+        <v>28240</v>
+      </c>
+      <c r="I108" t="n">
+        <v>2671</v>
+      </c>
+      <c r="J108" t="inlineStr">
+        <is>
+          <t>day</t>
+        </is>
+      </c>
+      <c r="K108" t="inlineStr">
+        <is>
+          <t>Bruce Wilson</t>
+        </is>
+      </c>
+      <c r="L108" t="inlineStr">
+        <is>
+          <t>bruce</t>
+        </is>
+      </c>
+      <c r="M108" t="inlineStr">
+        <is>
+          <t>wilson</t>
+        </is>
+      </c>
+      <c r="O108" t="inlineStr">
+        <is>
+          <t>male</t>
+        </is>
+      </c>
+      <c r="P108" t="n">
+        <v>38.8260509424163</v>
+      </c>
+      <c r="Q108" t="n">
+        <v>-77.0132524953315</v>
+      </c>
+      <c r="R108" t="inlineStr">
+        <is>
+          <t>ELMIRA STREET SW FROM MARTIN LUTHER KING JR AVENUE SW TO MARTIN LUTHER KING JR AVENUE SW</t>
+        </is>
+      </c>
+      <c r="S108" t="inlineStr">
+        <is>
+          <t>avon c  alexander</t>
+        </is>
+      </c>
+      <c r="T108" t="inlineStr">
+        <is>
+          <t>firearm</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109">
+        <f>MOD(IF($B109 = $B108, $A108, $A108 + 1), 2)</f>
+        <v/>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>100019803:0:0</t>
+        </is>
+      </c>
+      <c r="C109" t="n">
+        <v>1</v>
+      </c>
+      <c r="D109" t="inlineStr">
+        <is>
+          <t>woodward</t>
+        </is>
+      </c>
+      <c r="E109" t="n">
+        <v>100019803</v>
+      </c>
+      <c r="F109" t="inlineStr">
+        <is>
+          <t>100019803:0:0</t>
+        </is>
+      </c>
+      <c r="G109" t="n">
+        <v>2</v>
+      </c>
+      <c r="H109" s="3" t="n">
+        <v>28355</v>
+      </c>
+      <c r="I109" t="n">
+        <v>2786</v>
+      </c>
+      <c r="J109" t="inlineStr">
+        <is>
+          <t>day</t>
+        </is>
+      </c>
+      <c r="K109" t="inlineStr">
+        <is>
+          <t>Charles Hamilton Woodward</t>
+        </is>
+      </c>
+      <c r="L109" t="inlineStr">
+        <is>
+          <t>charles</t>
+        </is>
+      </c>
+      <c r="M109" t="inlineStr">
+        <is>
+          <t>woodward</t>
+        </is>
+      </c>
+      <c r="N109" t="n">
+        <v>24</v>
+      </c>
+      <c r="O109" t="inlineStr">
+        <is>
+          <t>male</t>
+        </is>
+      </c>
+      <c r="P109" t="n">
+        <v>38.8606803729819</v>
+      </c>
+      <c r="Q109" t="n">
+        <v>-76.9693260907099</v>
+      </c>
+      <c r="R109" t="inlineStr">
+        <is>
+          <t>2501 GOOD HOPE ROAD SE</t>
+        </is>
+      </c>
+      <c r="T109" t="inlineStr">
+        <is>
+          <t>firearm</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110">
+        <f>MOD(IF($B110 = $B109, $A109, $A109 + 1), 2)</f>
+        <v/>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>100016342:0:0</t>
+        </is>
+      </c>
+      <c r="C110" t="n">
+        <v>1</v>
+      </c>
+      <c r="D110" t="inlineStr">
+        <is>
+          <t>worthy</t>
+        </is>
+      </c>
+      <c r="E110" t="n">
+        <v>100016342</v>
+      </c>
+      <c r="F110" t="inlineStr">
+        <is>
+          <t>100016342:0:0</t>
+        </is>
+      </c>
+      <c r="G110" t="n">
+        <v>2</v>
+      </c>
+      <c r="H110" s="3" t="n">
+        <v>28336</v>
+      </c>
+      <c r="I110" t="n">
+        <v>2767</v>
+      </c>
+      <c r="J110" t="inlineStr">
+        <is>
+          <t>day</t>
+        </is>
+      </c>
+      <c r="K110" t="inlineStr">
+        <is>
+          <t>John Worthy</t>
+        </is>
+      </c>
+      <c r="L110" t="inlineStr">
+        <is>
+          <t>john</t>
+        </is>
+      </c>
+      <c r="M110" t="inlineStr">
+        <is>
+          <t>worthy</t>
+        </is>
+      </c>
+      <c r="N110" t="n">
+        <v>67</v>
+      </c>
+      <c r="O110" t="inlineStr">
+        <is>
+          <t>male</t>
+        </is>
+      </c>
+      <c r="P110" t="n">
+        <v>38.9056454536728</v>
+      </c>
+      <c r="Q110" t="n">
+        <v>-77.02399247492311</v>
+      </c>
+      <c r="R110" t="inlineStr">
+        <is>
+          <t>9TH STREET NW AND M STREET NW</t>
+        </is>
+      </c>
+      <c r="S110" t="inlineStr">
+        <is>
+          <t>mary gillespie</t>
+        </is>
+      </c>
+      <c r="T110" t="inlineStr">
+        <is>
+          <t>firearm</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111">
+        <f>MOD(IF($B111 = $B110, $A110, $A110 + 1), 2)</f>
+        <v/>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
           <t>100052572:0:0</t>
         </is>
       </c>
-      <c r="C108" t="n">
+      <c r="C111" t="n">
         <v>1</v>
       </c>
-      <c r="D108" t="inlineStr">
+      <c r="D111" t="inlineStr">
         <is>
           <t>wright</t>
         </is>
       </c>
-      <c r="E108" t="n">
+      <c r="E111" t="n">
         <v>100052572</v>
       </c>
-      <c r="F108" t="inlineStr">
+      <c r="F111" t="inlineStr">
         <is>
           <t>100052572:0:0</t>
         </is>
       </c>
-      <c r="G108" t="n">
-        <v>2</v>
-      </c>
-      <c r="H108" s="3" t="n">
+      <c r="G111" t="n">
+        <v>2</v>
+      </c>
+      <c r="H111" s="3" t="n">
         <v>28159</v>
       </c>
-      <c r="I108" t="n">
+      <c r="I111" t="n">
         <v>2590</v>
       </c>
-      <c r="J108" t="inlineStr">
-        <is>
-          <t>day</t>
-        </is>
-      </c>
-      <c r="K108" t="inlineStr">
+      <c r="J111" t="inlineStr">
+        <is>
+          <t>day</t>
+        </is>
+      </c>
+      <c r="K111" t="inlineStr">
         <is>
           <t>Lenora Wright</t>
         </is>
       </c>
-      <c r="L108" t="inlineStr">
+      <c r="L111" t="inlineStr">
         <is>
           <t>lenora</t>
         </is>
       </c>
-      <c r="M108" t="inlineStr">
+      <c r="M111" t="inlineStr">
         <is>
           <t>wright</t>
         </is>
       </c>
-      <c r="N108" t="n">
+      <c r="N111" t="n">
         <v>21</v>
       </c>
-      <c r="O108" t="inlineStr">
+      <c r="O111" t="inlineStr">
         <is>
           <t>female</t>
         </is>
       </c>
-      <c r="P108" t="n">
+      <c r="P111" t="n">
         <v>38.8796229150195</v>
       </c>
-      <c r="Q108" t="n">
+      <c r="Q111" t="n">
         <v>-76.9320514841373</v>
       </c>
-      <c r="R108" t="inlineStr">
+      <c r="R111" t="inlineStr">
         <is>
           <t>HANNA PLACE SE AND BENNING ROAD SE</t>
         </is>
       </c>
-      <c r="T108" t="inlineStr">
+      <c r="T111" t="inlineStr">
         <is>
           <t>strangulation</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A2:T108">
+  <conditionalFormatting sqref="A2:T111">
     <cfRule type="expression" priority="1" dxfId="0">
       <formula>$A2 = 0</formula>
     </cfRule>

</xml_diff>